<commit_message>
Update test artefacts to new format of fiscal years
</commit_message>
<xml_diff>
--- a/tests/artefacts/api/exports/activities_xlsx.xlsx
+++ b/tests/artefacts/api/exports/activities_xlsx.xlsx
@@ -420,7 +420,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:DH11"/>
+  <dimension ref="A1:DT11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -571,422 +571,482 @@
       </c>
       <c r="AC1" s="1" t="inlineStr">
         <is>
-          <t>2013 Q1 (MTEF)</t>
+          <t>FY2013 Q1 (MTEF)</t>
         </is>
       </c>
       <c r="AD1" s="1" t="inlineStr">
         <is>
-          <t>2013 Q2 (MTEF)</t>
+          <t>FY2013 Q2 (MTEF)</t>
         </is>
       </c>
       <c r="AE1" s="1" t="inlineStr">
         <is>
-          <t>2013 Q3 (MTEF)</t>
+          <t>FY2013 Q3 (MTEF)</t>
         </is>
       </c>
       <c r="AF1" s="1" t="inlineStr">
         <is>
-          <t>2013 Q4 (MTEF)</t>
+          <t>FY2013 Q4 (MTEF)</t>
         </is>
       </c>
       <c r="AG1" s="1" t="inlineStr">
         <is>
-          <t>2013 Q1 (D)</t>
+          <t>FY2014 Q1 (MTEF)</t>
         </is>
       </c>
       <c r="AH1" s="1" t="inlineStr">
         <is>
-          <t>2013 Q2 (D)</t>
+          <t>FY2014 Q2 (MTEF)</t>
         </is>
       </c>
       <c r="AI1" s="1" t="inlineStr">
         <is>
-          <t>2013 Q3 (D)</t>
+          <t>FY2014 Q3 (MTEF)</t>
         </is>
       </c>
       <c r="AJ1" s="1" t="inlineStr">
         <is>
-          <t>2013 Q4 (D)</t>
+          <t>FY2014 Q4 (MTEF)</t>
         </is>
       </c>
       <c r="AK1" s="1" t="inlineStr">
         <is>
-          <t>2014 Q1 (MTEF)</t>
+          <t>FY2015 Q1 (MTEF)</t>
         </is>
       </c>
       <c r="AL1" s="1" t="inlineStr">
         <is>
-          <t>2014 Q2 (MTEF)</t>
+          <t>FY2015 Q2 (MTEF)</t>
         </is>
       </c>
       <c r="AM1" s="1" t="inlineStr">
         <is>
-          <t>2014 Q3 (MTEF)</t>
+          <t>FY2015 Q3 (MTEF)</t>
         </is>
       </c>
       <c r="AN1" s="1" t="inlineStr">
         <is>
-          <t>2014 Q4 (MTEF)</t>
+          <t>FY2015 Q4 (MTEF)</t>
         </is>
       </c>
       <c r="AO1" s="1" t="inlineStr">
         <is>
-          <t>2014 Q1 (D)</t>
+          <t>FY2016 Q1 (MTEF)</t>
         </is>
       </c>
       <c r="AP1" s="1" t="inlineStr">
         <is>
-          <t>2014 Q2 (D)</t>
+          <t>FY2016 Q2 (MTEF)</t>
         </is>
       </c>
       <c r="AQ1" s="1" t="inlineStr">
         <is>
-          <t>2014 Q3 (D)</t>
+          <t>FY2016 Q3 (MTEF)</t>
         </is>
       </c>
       <c r="AR1" s="1" t="inlineStr">
         <is>
-          <t>2014 Q4 (D)</t>
+          <t>FY2016 Q4 (MTEF)</t>
         </is>
       </c>
       <c r="AS1" s="1" t="inlineStr">
         <is>
-          <t>2015 Q1 (MTEF)</t>
+          <t>FY2017 Q1 (MTEF)</t>
         </is>
       </c>
       <c r="AT1" s="1" t="inlineStr">
         <is>
-          <t>2015 Q2 (MTEF)</t>
+          <t>FY2017 Q2 (MTEF)</t>
         </is>
       </c>
       <c r="AU1" s="1" t="inlineStr">
         <is>
-          <t>2015 Q3 (MTEF)</t>
+          <t>FY2017 Q3 (MTEF)</t>
         </is>
       </c>
       <c r="AV1" s="1" t="inlineStr">
         <is>
-          <t>2015 Q4 (MTEF)</t>
+          <t>FY2017 Q4 (MTEF)</t>
         </is>
       </c>
       <c r="AW1" s="1" t="inlineStr">
         <is>
-          <t>2015 Q1 (D)</t>
+          <t>FY2018 Q1 (MTEF)</t>
         </is>
       </c>
       <c r="AX1" s="1" t="inlineStr">
         <is>
-          <t>2015 Q2 (D)</t>
+          <t>FY2018 Q2 (MTEF)</t>
         </is>
       </c>
       <c r="AY1" s="1" t="inlineStr">
         <is>
-          <t>2015 Q3 (D)</t>
+          <t>FY2018 Q3 (MTEF)</t>
         </is>
       </c>
       <c r="AZ1" s="1" t="inlineStr">
         <is>
-          <t>2015 Q4 (D)</t>
+          <t>FY2018 Q4 (MTEF)</t>
         </is>
       </c>
       <c r="BA1" s="1" t="inlineStr">
         <is>
-          <t>2016 Q1 (MTEF)</t>
+          <t>FY2019 Q1 (MTEF)</t>
         </is>
       </c>
       <c r="BB1" s="1" t="inlineStr">
         <is>
-          <t>2016 Q2 (MTEF)</t>
+          <t>FY2019 Q2 (MTEF)</t>
         </is>
       </c>
       <c r="BC1" s="1" t="inlineStr">
         <is>
-          <t>2016 Q3 (MTEF)</t>
+          <t>FY2019 Q3 (MTEF)</t>
         </is>
       </c>
       <c r="BD1" s="1" t="inlineStr">
         <is>
-          <t>2016 Q4 (MTEF)</t>
+          <t>FY2019 Q4 (MTEF)</t>
         </is>
       </c>
       <c r="BE1" s="1" t="inlineStr">
         <is>
-          <t>2016 Q1 (D)</t>
+          <t>FY2020 Q1 (MTEF)</t>
         </is>
       </c>
       <c r="BF1" s="1" t="inlineStr">
         <is>
-          <t>2016 Q2 (D)</t>
+          <t>FY2020 Q2 (MTEF)</t>
         </is>
       </c>
       <c r="BG1" s="1" t="inlineStr">
         <is>
-          <t>2016 Q3 (D)</t>
+          <t>FY2020 Q3 (MTEF)</t>
         </is>
       </c>
       <c r="BH1" s="1" t="inlineStr">
         <is>
-          <t>2016 Q4 (D)</t>
+          <t>FY2020 Q4 (MTEF)</t>
         </is>
       </c>
       <c r="BI1" s="1" t="inlineStr">
         <is>
-          <t>2017 Q1 (MTEF)</t>
+          <t>FY2021 Q1 (MTEF)</t>
         </is>
       </c>
       <c r="BJ1" s="1" t="inlineStr">
         <is>
-          <t>2017 Q2 (MTEF)</t>
+          <t>FY2021 Q2 (MTEF)</t>
         </is>
       </c>
       <c r="BK1" s="1" t="inlineStr">
         <is>
-          <t>2017 Q3 (MTEF)</t>
+          <t>FY2021 Q3 (MTEF)</t>
         </is>
       </c>
       <c r="BL1" s="1" t="inlineStr">
         <is>
-          <t>2017 Q4 (MTEF)</t>
+          <t>FY2021 Q4 (MTEF)</t>
         </is>
       </c>
       <c r="BM1" s="1" t="inlineStr">
         <is>
-          <t>2017 Q1 (D)</t>
+          <t>FY2022 Q1 (MTEF)</t>
         </is>
       </c>
       <c r="BN1" s="1" t="inlineStr">
         <is>
-          <t>2017 Q2 (D)</t>
+          <t>FY2022 Q2 (MTEF)</t>
         </is>
       </c>
       <c r="BO1" s="1" t="inlineStr">
         <is>
-          <t>2017 Q3 (D)</t>
+          <t>FY2022 Q3 (MTEF)</t>
         </is>
       </c>
       <c r="BP1" s="1" t="inlineStr">
         <is>
-          <t>2017 Q4 (D)</t>
+          <t>FY2022 Q4 (MTEF)</t>
         </is>
       </c>
       <c r="BQ1" s="1" t="inlineStr">
         <is>
-          <t>2018 Q1 (MTEF)</t>
+          <t>FY2023 Q1 (MTEF)</t>
         </is>
       </c>
       <c r="BR1" s="1" t="inlineStr">
         <is>
-          <t>2018 Q2 (MTEF)</t>
+          <t>FY2023 Q2 (MTEF)</t>
         </is>
       </c>
       <c r="BS1" s="1" t="inlineStr">
         <is>
-          <t>2018 Q3 (MTEF)</t>
+          <t>FY2023 Q3 (MTEF)</t>
         </is>
       </c>
       <c r="BT1" s="1" t="inlineStr">
         <is>
-          <t>2018 Q4 (MTEF)</t>
+          <t>FY2023 Q4 (MTEF)</t>
         </is>
       </c>
       <c r="BU1" s="1" t="inlineStr">
         <is>
-          <t>2018 Q1 (D)</t>
+          <t>FY2024 Q1 (MTEF)</t>
         </is>
       </c>
       <c r="BV1" s="1" t="inlineStr">
         <is>
-          <t>2018 Q2 (D)</t>
+          <t>FY2024 Q2 (MTEF)</t>
         </is>
       </c>
       <c r="BW1" s="1" t="inlineStr">
         <is>
-          <t>2018 Q3 (D)</t>
+          <t>FY2024 Q3 (MTEF)</t>
         </is>
       </c>
       <c r="BX1" s="1" t="inlineStr">
         <is>
-          <t>2018 Q4 (D)</t>
+          <t>FY2024 Q4 (MTEF)</t>
         </is>
       </c>
       <c r="BY1" s="1" t="inlineStr">
         <is>
-          <t>2019 Q1 (MTEF)</t>
+          <t>FY2013 Q1 (D)</t>
         </is>
       </c>
       <c r="BZ1" s="1" t="inlineStr">
         <is>
-          <t>2019 Q2 (MTEF)</t>
+          <t>FY2013 Q2 (D)</t>
         </is>
       </c>
       <c r="CA1" s="1" t="inlineStr">
         <is>
-          <t>2019 Q3 (MTEF)</t>
+          <t>FY2013 Q3 (D)</t>
         </is>
       </c>
       <c r="CB1" s="1" t="inlineStr">
         <is>
-          <t>2019 Q4 (MTEF)</t>
+          <t>FY2013 Q4 (D)</t>
         </is>
       </c>
       <c r="CC1" s="1" t="inlineStr">
         <is>
-          <t>2019 Q1 (D)</t>
+          <t>FY2014 Q1 (D)</t>
         </is>
       </c>
       <c r="CD1" s="1" t="inlineStr">
         <is>
-          <t>2019 Q2 (D)</t>
+          <t>FY2014 Q2 (D)</t>
         </is>
       </c>
       <c r="CE1" s="1" t="inlineStr">
         <is>
-          <t>2019 Q3 (D)</t>
+          <t>FY2014 Q3 (D)</t>
         </is>
       </c>
       <c r="CF1" s="1" t="inlineStr">
         <is>
-          <t>2019 Q4 (D)</t>
+          <t>FY2014 Q4 (D)</t>
         </is>
       </c>
       <c r="CG1" s="1" t="inlineStr">
         <is>
-          <t>2020 Q1 (MTEF)</t>
+          <t>FY2015 Q1 (D)</t>
         </is>
       </c>
       <c r="CH1" s="1" t="inlineStr">
         <is>
-          <t>2020 Q2 (MTEF)</t>
+          <t>FY2015 Q2 (D)</t>
         </is>
       </c>
       <c r="CI1" s="1" t="inlineStr">
         <is>
-          <t>2020 Q3 (MTEF)</t>
+          <t>FY2015 Q3 (D)</t>
         </is>
       </c>
       <c r="CJ1" s="1" t="inlineStr">
         <is>
-          <t>2020 Q4 (MTEF)</t>
+          <t>FY2015 Q4 (D)</t>
         </is>
       </c>
       <c r="CK1" s="1" t="inlineStr">
         <is>
-          <t>2020 Q1 (D)</t>
+          <t>FY2016 Q1 (D)</t>
         </is>
       </c>
       <c r="CL1" s="1" t="inlineStr">
         <is>
-          <t>2020 Q2 (D)</t>
+          <t>FY2016 Q2 (D)</t>
         </is>
       </c>
       <c r="CM1" s="1" t="inlineStr">
         <is>
-          <t>2020 Q3 (D)</t>
+          <t>FY2016 Q3 (D)</t>
         </is>
       </c>
       <c r="CN1" s="1" t="inlineStr">
         <is>
-          <t>2020 Q4 (D)</t>
+          <t>FY2016 Q4 (D)</t>
         </is>
       </c>
       <c r="CO1" s="1" t="inlineStr">
         <is>
-          <t>2021 Q1 (MTEF)</t>
+          <t>FY2017 Q1 (D)</t>
         </is>
       </c>
       <c r="CP1" s="1" t="inlineStr">
         <is>
-          <t>2021 Q2 (MTEF)</t>
+          <t>FY2017 Q2 (D)</t>
         </is>
       </c>
       <c r="CQ1" s="1" t="inlineStr">
         <is>
-          <t>2021 Q3 (MTEF)</t>
+          <t>FY2017 Q3 (D)</t>
         </is>
       </c>
       <c r="CR1" s="1" t="inlineStr">
         <is>
-          <t>2021 Q4 (MTEF)</t>
+          <t>FY2017 Q4 (D)</t>
         </is>
       </c>
       <c r="CS1" s="1" t="inlineStr">
         <is>
-          <t>2021 Q1 (D)</t>
+          <t>FY2018 Q1 (D)</t>
         </is>
       </c>
       <c r="CT1" s="1" t="inlineStr">
         <is>
-          <t>2021 Q2 (D)</t>
+          <t>FY2018 Q2 (D)</t>
         </is>
       </c>
       <c r="CU1" s="1" t="inlineStr">
         <is>
-          <t>2021 Q3 (D)</t>
+          <t>FY2018 Q3 (D)</t>
         </is>
       </c>
       <c r="CV1" s="1" t="inlineStr">
         <is>
-          <t>2021 Q4 (D)</t>
+          <t>FY2018 Q4 (D)</t>
         </is>
       </c>
       <c r="CW1" s="1" t="inlineStr">
         <is>
-          <t>2022 Q1 (MTEF)</t>
+          <t>FY2019 Q1 (D)</t>
         </is>
       </c>
       <c r="CX1" s="1" t="inlineStr">
         <is>
-          <t>2022 Q2 (MTEF)</t>
+          <t>FY2019 Q2 (D)</t>
         </is>
       </c>
       <c r="CY1" s="1" t="inlineStr">
         <is>
-          <t>2022 Q3 (MTEF)</t>
+          <t>FY2019 Q3 (D)</t>
         </is>
       </c>
       <c r="CZ1" s="1" t="inlineStr">
         <is>
-          <t>2022 Q4 (MTEF)</t>
+          <t>FY2019 Q4 (D)</t>
         </is>
       </c>
       <c r="DA1" s="1" t="inlineStr">
         <is>
-          <t>2023 Q1 (MTEF)</t>
+          <t>FY2020 Q1 (D)</t>
         </is>
       </c>
       <c r="DB1" s="1" t="inlineStr">
         <is>
-          <t>2023 Q2 (MTEF)</t>
+          <t>FY2020 Q2 (D)</t>
         </is>
       </c>
       <c r="DC1" s="1" t="inlineStr">
         <is>
-          <t>2023 Q3 (MTEF)</t>
+          <t>FY2020 Q3 (D)</t>
         </is>
       </c>
       <c r="DD1" s="1" t="inlineStr">
         <is>
-          <t>2023 Q4 (MTEF)</t>
+          <t>FY2020 Q4 (D)</t>
         </is>
       </c>
       <c r="DE1" s="1" t="inlineStr">
         <is>
-          <t>2024 Q1 (MTEF)</t>
+          <t>FY2021 Q1 (D)</t>
         </is>
       </c>
       <c r="DF1" s="1" t="inlineStr">
         <is>
-          <t>2024 Q2 (MTEF)</t>
+          <t>FY2021 Q2 (D)</t>
         </is>
       </c>
       <c r="DG1" s="1" t="inlineStr">
         <is>
-          <t>2024 Q3 (MTEF)</t>
+          <t>FY2021 Q3 (D)</t>
         </is>
       </c>
       <c r="DH1" s="1" t="inlineStr">
         <is>
-          <t>2024 Q4 (MTEF)</t>
+          <t>FY2021 Q4 (D)</t>
+        </is>
+      </c>
+      <c r="DI1" s="1" t="inlineStr">
+        <is>
+          <t>FY2022 Q1 (D)</t>
+        </is>
+      </c>
+      <c r="DJ1" s="1" t="inlineStr">
+        <is>
+          <t>FY2022 Q2 (D)</t>
+        </is>
+      </c>
+      <c r="DK1" s="1" t="inlineStr">
+        <is>
+          <t>FY2022 Q3 (D)</t>
+        </is>
+      </c>
+      <c r="DL1" s="1" t="inlineStr">
+        <is>
+          <t>FY2022 Q4 (D)</t>
+        </is>
+      </c>
+      <c r="DM1" s="1" t="inlineStr">
+        <is>
+          <t>FY2023 Q1 (D)</t>
+        </is>
+      </c>
+      <c r="DN1" s="1" t="inlineStr">
+        <is>
+          <t>FY2023 Q2 (D)</t>
+        </is>
+      </c>
+      <c r="DO1" s="1" t="inlineStr">
+        <is>
+          <t>FY2023 Q3 (D)</t>
+        </is>
+      </c>
+      <c r="DP1" s="1" t="inlineStr">
+        <is>
+          <t>FY2023 Q4 (D)</t>
+        </is>
+      </c>
+      <c r="DQ1" s="1" t="inlineStr">
+        <is>
+          <t>FY2024 Q1 (D)</t>
+        </is>
+      </c>
+      <c r="DR1" s="1" t="inlineStr">
+        <is>
+          <t>FY2024 Q2 (D)</t>
+        </is>
+      </c>
+      <c r="DS1" s="1" t="inlineStr">
+        <is>
+          <t>FY2024 Q3 (D)</t>
+        </is>
+      </c>
+      <c r="DT1" s="1" t="inlineStr">
+        <is>
+          <t>FY2024 Q4 (D)</t>
         </is>
       </c>
     </row>
@@ -1057,7 +1117,7 @@
       <c r="Z2" t="inlineStr"/>
       <c r="AA2" t="inlineStr"/>
       <c r="AB2" s="2" t="n">
-        <v>44313</v>
+        <v>44420</v>
       </c>
       <c r="AC2" t="n">
         <v>0</v>
@@ -1120,16 +1180,16 @@
         <v>0</v>
       </c>
       <c r="AW2" t="n">
-        <v>0</v>
+        <v>250</v>
       </c>
       <c r="AX2" t="n">
-        <v>0</v>
+        <v>250</v>
       </c>
       <c r="AY2" t="n">
-        <v>0</v>
+        <v>250</v>
       </c>
       <c r="AZ2" t="n">
-        <v>0</v>
+        <v>250</v>
       </c>
       <c r="BA2" t="n">
         <v>0</v>
@@ -1180,16 +1240,16 @@
         <v>0</v>
       </c>
       <c r="BQ2" t="n">
-        <v>250</v>
+        <v>0</v>
       </c>
       <c r="BR2" t="n">
-        <v>250</v>
+        <v>0</v>
       </c>
       <c r="BS2" t="n">
-        <v>250</v>
+        <v>0</v>
       </c>
       <c r="BT2" t="n">
-        <v>250</v>
+        <v>0</v>
       </c>
       <c r="BU2" t="n">
         <v>0</v>
@@ -1216,68 +1276,68 @@
         <v>0</v>
       </c>
       <c r="CC2" t="n">
+        <v>0</v>
+      </c>
+      <c r="CD2" t="n">
+        <v>0</v>
+      </c>
+      <c r="CE2" t="n">
+        <v>0</v>
+      </c>
+      <c r="CF2" t="n">
+        <v>0</v>
+      </c>
+      <c r="CG2" t="n">
+        <v>0</v>
+      </c>
+      <c r="CH2" t="n">
+        <v>0</v>
+      </c>
+      <c r="CI2" t="n">
+        <v>0</v>
+      </c>
+      <c r="CJ2" t="n">
+        <v>0</v>
+      </c>
+      <c r="CK2" t="n">
+        <v>0</v>
+      </c>
+      <c r="CL2" t="n">
+        <v>0</v>
+      </c>
+      <c r="CM2" t="n">
+        <v>0</v>
+      </c>
+      <c r="CN2" t="n">
+        <v>0</v>
+      </c>
+      <c r="CO2" t="n">
+        <v>0</v>
+      </c>
+      <c r="CP2" t="n">
+        <v>0</v>
+      </c>
+      <c r="CQ2" t="n">
+        <v>0</v>
+      </c>
+      <c r="CR2" t="n">
+        <v>0</v>
+      </c>
+      <c r="CS2" t="n">
+        <v>0</v>
+      </c>
+      <c r="CT2" t="n">
+        <v>0</v>
+      </c>
+      <c r="CU2" t="n">
+        <v>0</v>
+      </c>
+      <c r="CV2" t="n">
+        <v>0</v>
+      </c>
+      <c r="CW2" t="n">
         <v>100</v>
       </c>
-      <c r="CD2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CE2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CF2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CG2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CH2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CI2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CJ2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CK2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CL2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CM2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CN2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CO2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CP2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CQ2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CT2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CU2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CV2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CW2" t="n">
-        <v>0</v>
-      </c>
       <c r="CX2" t="n">
         <v>0</v>
       </c>
@@ -1309,6 +1369,42 @@
         <v>0</v>
       </c>
       <c r="DH2" t="n">
+        <v>0</v>
+      </c>
+      <c r="DI2" t="n">
+        <v>0</v>
+      </c>
+      <c r="DJ2" t="n">
+        <v>0</v>
+      </c>
+      <c r="DK2" t="n">
+        <v>0</v>
+      </c>
+      <c r="DL2" t="n">
+        <v>0</v>
+      </c>
+      <c r="DM2" t="n">
+        <v>0</v>
+      </c>
+      <c r="DN2" t="n">
+        <v>0</v>
+      </c>
+      <c r="DO2" t="n">
+        <v>0</v>
+      </c>
+      <c r="DP2" t="n">
+        <v>0</v>
+      </c>
+      <c r="DQ2" t="n">
+        <v>0</v>
+      </c>
+      <c r="DR2" t="n">
+        <v>0</v>
+      </c>
+      <c r="DS2" t="n">
+        <v>0</v>
+      </c>
+      <c r="DT2" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1379,7 +1475,7 @@
       <c r="Z3" t="inlineStr"/>
       <c r="AA3" t="inlineStr"/>
       <c r="AB3" s="2" t="n">
-        <v>44313</v>
+        <v>44420</v>
       </c>
       <c r="AC3" t="n">
         <v>0</v>
@@ -1442,16 +1538,16 @@
         <v>0</v>
       </c>
       <c r="AW3" t="n">
-        <v>0</v>
+        <v>500</v>
       </c>
       <c r="AX3" t="n">
-        <v>0</v>
+        <v>500</v>
       </c>
       <c r="AY3" t="n">
-        <v>0</v>
+        <v>500</v>
       </c>
       <c r="AZ3" t="n">
-        <v>0</v>
+        <v>500</v>
       </c>
       <c r="BA3" t="n">
         <v>0</v>
@@ -1502,16 +1598,16 @@
         <v>0</v>
       </c>
       <c r="BQ3" t="n">
-        <v>500</v>
+        <v>0</v>
       </c>
       <c r="BR3" t="n">
-        <v>500</v>
+        <v>0</v>
       </c>
       <c r="BS3" t="n">
-        <v>500</v>
+        <v>0</v>
       </c>
       <c r="BT3" t="n">
-        <v>500</v>
+        <v>0</v>
       </c>
       <c r="BU3" t="n">
         <v>0</v>
@@ -1538,68 +1634,68 @@
         <v>0</v>
       </c>
       <c r="CC3" t="n">
+        <v>0</v>
+      </c>
+      <c r="CD3" t="n">
+        <v>0</v>
+      </c>
+      <c r="CE3" t="n">
+        <v>0</v>
+      </c>
+      <c r="CF3" t="n">
+        <v>0</v>
+      </c>
+      <c r="CG3" t="n">
+        <v>0</v>
+      </c>
+      <c r="CH3" t="n">
+        <v>0</v>
+      </c>
+      <c r="CI3" t="n">
+        <v>0</v>
+      </c>
+      <c r="CJ3" t="n">
+        <v>0</v>
+      </c>
+      <c r="CK3" t="n">
+        <v>0</v>
+      </c>
+      <c r="CL3" t="n">
+        <v>0</v>
+      </c>
+      <c r="CM3" t="n">
+        <v>0</v>
+      </c>
+      <c r="CN3" t="n">
+        <v>0</v>
+      </c>
+      <c r="CO3" t="n">
+        <v>0</v>
+      </c>
+      <c r="CP3" t="n">
+        <v>0</v>
+      </c>
+      <c r="CQ3" t="n">
+        <v>0</v>
+      </c>
+      <c r="CR3" t="n">
+        <v>0</v>
+      </c>
+      <c r="CS3" t="n">
+        <v>0</v>
+      </c>
+      <c r="CT3" t="n">
+        <v>0</v>
+      </c>
+      <c r="CU3" t="n">
+        <v>0</v>
+      </c>
+      <c r="CV3" t="n">
+        <v>0</v>
+      </c>
+      <c r="CW3" t="n">
         <v>2000</v>
       </c>
-      <c r="CD3" t="n">
-        <v>0</v>
-      </c>
-      <c r="CE3" t="n">
-        <v>0</v>
-      </c>
-      <c r="CF3" t="n">
-        <v>0</v>
-      </c>
-      <c r="CG3" t="n">
-        <v>0</v>
-      </c>
-      <c r="CH3" t="n">
-        <v>0</v>
-      </c>
-      <c r="CI3" t="n">
-        <v>0</v>
-      </c>
-      <c r="CJ3" t="n">
-        <v>0</v>
-      </c>
-      <c r="CK3" t="n">
-        <v>0</v>
-      </c>
-      <c r="CL3" t="n">
-        <v>0</v>
-      </c>
-      <c r="CM3" t="n">
-        <v>0</v>
-      </c>
-      <c r="CN3" t="n">
-        <v>0</v>
-      </c>
-      <c r="CO3" t="n">
-        <v>0</v>
-      </c>
-      <c r="CP3" t="n">
-        <v>0</v>
-      </c>
-      <c r="CQ3" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR3" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS3" t="n">
-        <v>0</v>
-      </c>
-      <c r="CT3" t="n">
-        <v>0</v>
-      </c>
-      <c r="CU3" t="n">
-        <v>0</v>
-      </c>
-      <c r="CV3" t="n">
-        <v>0</v>
-      </c>
-      <c r="CW3" t="n">
-        <v>0</v>
-      </c>
       <c r="CX3" t="n">
         <v>0</v>
       </c>
@@ -1631,6 +1727,42 @@
         <v>0</v>
       </c>
       <c r="DH3" t="n">
+        <v>0</v>
+      </c>
+      <c r="DI3" t="n">
+        <v>0</v>
+      </c>
+      <c r="DJ3" t="n">
+        <v>0</v>
+      </c>
+      <c r="DK3" t="n">
+        <v>0</v>
+      </c>
+      <c r="DL3" t="n">
+        <v>0</v>
+      </c>
+      <c r="DM3" t="n">
+        <v>0</v>
+      </c>
+      <c r="DN3" t="n">
+        <v>0</v>
+      </c>
+      <c r="DO3" t="n">
+        <v>0</v>
+      </c>
+      <c r="DP3" t="n">
+        <v>0</v>
+      </c>
+      <c r="DQ3" t="n">
+        <v>0</v>
+      </c>
+      <c r="DR3" t="n">
+        <v>0</v>
+      </c>
+      <c r="DS3" t="n">
+        <v>0</v>
+      </c>
+      <c r="DT3" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1701,7 +1833,7 @@
       <c r="Z4" t="inlineStr"/>
       <c r="AA4" t="inlineStr"/>
       <c r="AB4" s="2" t="n">
-        <v>44313</v>
+        <v>44420</v>
       </c>
       <c r="AC4" t="n">
         <v>0</v>
@@ -1764,16 +1896,16 @@
         <v>0</v>
       </c>
       <c r="AW4" t="n">
-        <v>0</v>
+        <v>1250</v>
       </c>
       <c r="AX4" t="n">
-        <v>0</v>
+        <v>1250</v>
       </c>
       <c r="AY4" t="n">
-        <v>0</v>
+        <v>1250</v>
       </c>
       <c r="AZ4" t="n">
-        <v>0</v>
+        <v>1250</v>
       </c>
       <c r="BA4" t="n">
         <v>0</v>
@@ -1824,16 +1956,16 @@
         <v>0</v>
       </c>
       <c r="BQ4" t="n">
-        <v>1250</v>
+        <v>0</v>
       </c>
       <c r="BR4" t="n">
-        <v>1250</v>
+        <v>0</v>
       </c>
       <c r="BS4" t="n">
-        <v>1250</v>
+        <v>0</v>
       </c>
       <c r="BT4" t="n">
-        <v>1250</v>
+        <v>0</v>
       </c>
       <c r="BU4" t="n">
         <v>0</v>
@@ -1860,68 +1992,68 @@
         <v>0</v>
       </c>
       <c r="CC4" t="n">
+        <v>0</v>
+      </c>
+      <c r="CD4" t="n">
+        <v>0</v>
+      </c>
+      <c r="CE4" t="n">
+        <v>0</v>
+      </c>
+      <c r="CF4" t="n">
+        <v>0</v>
+      </c>
+      <c r="CG4" t="n">
+        <v>0</v>
+      </c>
+      <c r="CH4" t="n">
+        <v>0</v>
+      </c>
+      <c r="CI4" t="n">
+        <v>0</v>
+      </c>
+      <c r="CJ4" t="n">
+        <v>0</v>
+      </c>
+      <c r="CK4" t="n">
+        <v>0</v>
+      </c>
+      <c r="CL4" t="n">
+        <v>0</v>
+      </c>
+      <c r="CM4" t="n">
+        <v>0</v>
+      </c>
+      <c r="CN4" t="n">
+        <v>0</v>
+      </c>
+      <c r="CO4" t="n">
+        <v>0</v>
+      </c>
+      <c r="CP4" t="n">
+        <v>0</v>
+      </c>
+      <c r="CQ4" t="n">
+        <v>0</v>
+      </c>
+      <c r="CR4" t="n">
+        <v>0</v>
+      </c>
+      <c r="CS4" t="n">
+        <v>0</v>
+      </c>
+      <c r="CT4" t="n">
+        <v>0</v>
+      </c>
+      <c r="CU4" t="n">
+        <v>0</v>
+      </c>
+      <c r="CV4" t="n">
+        <v>0</v>
+      </c>
+      <c r="CW4" t="n">
         <v>300</v>
       </c>
-      <c r="CD4" t="n">
-        <v>0</v>
-      </c>
-      <c r="CE4" t="n">
-        <v>0</v>
-      </c>
-      <c r="CF4" t="n">
-        <v>0</v>
-      </c>
-      <c r="CG4" t="n">
-        <v>0</v>
-      </c>
-      <c r="CH4" t="n">
-        <v>0</v>
-      </c>
-      <c r="CI4" t="n">
-        <v>0</v>
-      </c>
-      <c r="CJ4" t="n">
-        <v>0</v>
-      </c>
-      <c r="CK4" t="n">
-        <v>0</v>
-      </c>
-      <c r="CL4" t="n">
-        <v>0</v>
-      </c>
-      <c r="CM4" t="n">
-        <v>0</v>
-      </c>
-      <c r="CN4" t="n">
-        <v>0</v>
-      </c>
-      <c r="CO4" t="n">
-        <v>0</v>
-      </c>
-      <c r="CP4" t="n">
-        <v>0</v>
-      </c>
-      <c r="CQ4" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR4" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS4" t="n">
-        <v>0</v>
-      </c>
-      <c r="CT4" t="n">
-        <v>0</v>
-      </c>
-      <c r="CU4" t="n">
-        <v>0</v>
-      </c>
-      <c r="CV4" t="n">
-        <v>0</v>
-      </c>
-      <c r="CW4" t="n">
-        <v>0</v>
-      </c>
       <c r="CX4" t="n">
         <v>0</v>
       </c>
@@ -1953,6 +2085,42 @@
         <v>0</v>
       </c>
       <c r="DH4" t="n">
+        <v>0</v>
+      </c>
+      <c r="DI4" t="n">
+        <v>0</v>
+      </c>
+      <c r="DJ4" t="n">
+        <v>0</v>
+      </c>
+      <c r="DK4" t="n">
+        <v>0</v>
+      </c>
+      <c r="DL4" t="n">
+        <v>0</v>
+      </c>
+      <c r="DM4" t="n">
+        <v>0</v>
+      </c>
+      <c r="DN4" t="n">
+        <v>0</v>
+      </c>
+      <c r="DO4" t="n">
+        <v>0</v>
+      </c>
+      <c r="DP4" t="n">
+        <v>0</v>
+      </c>
+      <c r="DQ4" t="n">
+        <v>0</v>
+      </c>
+      <c r="DR4" t="n">
+        <v>0</v>
+      </c>
+      <c r="DS4" t="n">
+        <v>0</v>
+      </c>
+      <c r="DT4" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2023,7 +2191,7 @@
       <c r="Z5" t="inlineStr"/>
       <c r="AA5" t="inlineStr"/>
       <c r="AB5" s="2" t="n">
-        <v>44313</v>
+        <v>44420</v>
       </c>
       <c r="AC5" t="n">
         <v>0</v>
@@ -2086,16 +2254,16 @@
         <v>0</v>
       </c>
       <c r="AW5" t="n">
-        <v>0</v>
+        <v>750</v>
       </c>
       <c r="AX5" t="n">
-        <v>0</v>
+        <v>750</v>
       </c>
       <c r="AY5" t="n">
-        <v>0</v>
+        <v>750</v>
       </c>
       <c r="AZ5" t="n">
-        <v>0</v>
+        <v>750</v>
       </c>
       <c r="BA5" t="n">
         <v>0</v>
@@ -2146,16 +2314,16 @@
         <v>0</v>
       </c>
       <c r="BQ5" t="n">
-        <v>750</v>
+        <v>0</v>
       </c>
       <c r="BR5" t="n">
-        <v>750</v>
+        <v>0</v>
       </c>
       <c r="BS5" t="n">
-        <v>750</v>
+        <v>0</v>
       </c>
       <c r="BT5" t="n">
-        <v>750</v>
+        <v>0</v>
       </c>
       <c r="BU5" t="n">
         <v>0</v>
@@ -2182,68 +2350,68 @@
         <v>0</v>
       </c>
       <c r="CC5" t="n">
+        <v>0</v>
+      </c>
+      <c r="CD5" t="n">
+        <v>0</v>
+      </c>
+      <c r="CE5" t="n">
+        <v>0</v>
+      </c>
+      <c r="CF5" t="n">
+        <v>0</v>
+      </c>
+      <c r="CG5" t="n">
+        <v>0</v>
+      </c>
+      <c r="CH5" t="n">
+        <v>0</v>
+      </c>
+      <c r="CI5" t="n">
+        <v>0</v>
+      </c>
+      <c r="CJ5" t="n">
+        <v>0</v>
+      </c>
+      <c r="CK5" t="n">
+        <v>0</v>
+      </c>
+      <c r="CL5" t="n">
+        <v>0</v>
+      </c>
+      <c r="CM5" t="n">
+        <v>0</v>
+      </c>
+      <c r="CN5" t="n">
+        <v>0</v>
+      </c>
+      <c r="CO5" t="n">
+        <v>0</v>
+      </c>
+      <c r="CP5" t="n">
+        <v>0</v>
+      </c>
+      <c r="CQ5" t="n">
+        <v>0</v>
+      </c>
+      <c r="CR5" t="n">
+        <v>0</v>
+      </c>
+      <c r="CS5" t="n">
+        <v>0</v>
+      </c>
+      <c r="CT5" t="n">
+        <v>0</v>
+      </c>
+      <c r="CU5" t="n">
+        <v>0</v>
+      </c>
+      <c r="CV5" t="n">
+        <v>0</v>
+      </c>
+      <c r="CW5" t="n">
         <v>400</v>
       </c>
-      <c r="CD5" t="n">
-        <v>0</v>
-      </c>
-      <c r="CE5" t="n">
-        <v>0</v>
-      </c>
-      <c r="CF5" t="n">
-        <v>0</v>
-      </c>
-      <c r="CG5" t="n">
-        <v>0</v>
-      </c>
-      <c r="CH5" t="n">
-        <v>0</v>
-      </c>
-      <c r="CI5" t="n">
-        <v>0</v>
-      </c>
-      <c r="CJ5" t="n">
-        <v>0</v>
-      </c>
-      <c r="CK5" t="n">
-        <v>0</v>
-      </c>
-      <c r="CL5" t="n">
-        <v>0</v>
-      </c>
-      <c r="CM5" t="n">
-        <v>0</v>
-      </c>
-      <c r="CN5" t="n">
-        <v>0</v>
-      </c>
-      <c r="CO5" t="n">
-        <v>0</v>
-      </c>
-      <c r="CP5" t="n">
-        <v>0</v>
-      </c>
-      <c r="CQ5" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR5" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS5" t="n">
-        <v>0</v>
-      </c>
-      <c r="CT5" t="n">
-        <v>0</v>
-      </c>
-      <c r="CU5" t="n">
-        <v>0</v>
-      </c>
-      <c r="CV5" t="n">
-        <v>0</v>
-      </c>
-      <c r="CW5" t="n">
-        <v>0</v>
-      </c>
       <c r="CX5" t="n">
         <v>0</v>
       </c>
@@ -2275,6 +2443,42 @@
         <v>0</v>
       </c>
       <c r="DH5" t="n">
+        <v>0</v>
+      </c>
+      <c r="DI5" t="n">
+        <v>0</v>
+      </c>
+      <c r="DJ5" t="n">
+        <v>0</v>
+      </c>
+      <c r="DK5" t="n">
+        <v>0</v>
+      </c>
+      <c r="DL5" t="n">
+        <v>0</v>
+      </c>
+      <c r="DM5" t="n">
+        <v>0</v>
+      </c>
+      <c r="DN5" t="n">
+        <v>0</v>
+      </c>
+      <c r="DO5" t="n">
+        <v>0</v>
+      </c>
+      <c r="DP5" t="n">
+        <v>0</v>
+      </c>
+      <c r="DQ5" t="n">
+        <v>0</v>
+      </c>
+      <c r="DR5" t="n">
+        <v>0</v>
+      </c>
+      <c r="DS5" t="n">
+        <v>0</v>
+      </c>
+      <c r="DT5" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2345,7 +2549,7 @@
       <c r="Z6" t="inlineStr"/>
       <c r="AA6" t="inlineStr"/>
       <c r="AB6" s="2" t="n">
-        <v>44313</v>
+        <v>44420</v>
       </c>
       <c r="AC6" t="n">
         <v>0</v>
@@ -2408,16 +2612,16 @@
         <v>0</v>
       </c>
       <c r="AW6" t="n">
-        <v>0</v>
+        <v>5000</v>
       </c>
       <c r="AX6" t="n">
-        <v>0</v>
+        <v>5000</v>
       </c>
       <c r="AY6" t="n">
-        <v>0</v>
+        <v>5000</v>
       </c>
       <c r="AZ6" t="n">
-        <v>0</v>
+        <v>5000</v>
       </c>
       <c r="BA6" t="n">
         <v>0</v>
@@ -2468,104 +2672,104 @@
         <v>0</v>
       </c>
       <c r="BQ6" t="n">
+        <v>0</v>
+      </c>
+      <c r="BR6" t="n">
+        <v>0</v>
+      </c>
+      <c r="BS6" t="n">
+        <v>0</v>
+      </c>
+      <c r="BT6" t="n">
+        <v>0</v>
+      </c>
+      <c r="BU6" t="n">
+        <v>0</v>
+      </c>
+      <c r="BV6" t="n">
+        <v>0</v>
+      </c>
+      <c r="BW6" t="n">
+        <v>0</v>
+      </c>
+      <c r="BX6" t="n">
+        <v>0</v>
+      </c>
+      <c r="BY6" t="n">
+        <v>0</v>
+      </c>
+      <c r="BZ6" t="n">
+        <v>0</v>
+      </c>
+      <c r="CA6" t="n">
+        <v>0</v>
+      </c>
+      <c r="CB6" t="n">
+        <v>0</v>
+      </c>
+      <c r="CC6" t="n">
+        <v>0</v>
+      </c>
+      <c r="CD6" t="n">
+        <v>0</v>
+      </c>
+      <c r="CE6" t="n">
+        <v>0</v>
+      </c>
+      <c r="CF6" t="n">
+        <v>0</v>
+      </c>
+      <c r="CG6" t="n">
+        <v>0</v>
+      </c>
+      <c r="CH6" t="n">
+        <v>0</v>
+      </c>
+      <c r="CI6" t="n">
+        <v>0</v>
+      </c>
+      <c r="CJ6" t="n">
+        <v>0</v>
+      </c>
+      <c r="CK6" t="n">
+        <v>0</v>
+      </c>
+      <c r="CL6" t="n">
+        <v>0</v>
+      </c>
+      <c r="CM6" t="n">
+        <v>0</v>
+      </c>
+      <c r="CN6" t="n">
+        <v>0</v>
+      </c>
+      <c r="CO6" t="n">
+        <v>0</v>
+      </c>
+      <c r="CP6" t="n">
+        <v>0</v>
+      </c>
+      <c r="CQ6" t="n">
+        <v>0</v>
+      </c>
+      <c r="CR6" t="n">
+        <v>0</v>
+      </c>
+      <c r="CS6" t="n">
+        <v>0</v>
+      </c>
+      <c r="CT6" t="n">
+        <v>0</v>
+      </c>
+      <c r="CU6" t="n">
+        <v>0</v>
+      </c>
+      <c r="CV6" t="n">
+        <v>0</v>
+      </c>
+      <c r="CW6" t="n">
         <v>5000</v>
       </c>
-      <c r="BR6" t="n">
-        <v>5000</v>
-      </c>
-      <c r="BS6" t="n">
-        <v>5000</v>
-      </c>
-      <c r="BT6" t="n">
-        <v>5000</v>
-      </c>
-      <c r="BU6" t="n">
-        <v>0</v>
-      </c>
-      <c r="BV6" t="n">
-        <v>0</v>
-      </c>
-      <c r="BW6" t="n">
-        <v>0</v>
-      </c>
-      <c r="BX6" t="n">
-        <v>0</v>
-      </c>
-      <c r="BY6" t="n">
-        <v>0</v>
-      </c>
-      <c r="BZ6" t="n">
-        <v>0</v>
-      </c>
-      <c r="CA6" t="n">
-        <v>0</v>
-      </c>
-      <c r="CB6" t="n">
-        <v>0</v>
-      </c>
-      <c r="CC6" t="n">
-        <v>5000</v>
-      </c>
-      <c r="CD6" t="n">
-        <v>0</v>
-      </c>
-      <c r="CE6" t="n">
-        <v>0</v>
-      </c>
-      <c r="CF6" t="n">
-        <v>0</v>
-      </c>
-      <c r="CG6" t="n">
-        <v>0</v>
-      </c>
-      <c r="CH6" t="n">
-        <v>0</v>
-      </c>
-      <c r="CI6" t="n">
-        <v>0</v>
-      </c>
-      <c r="CJ6" t="n">
-        <v>0</v>
-      </c>
-      <c r="CK6" t="n">
-        <v>0</v>
-      </c>
-      <c r="CL6" t="n">
-        <v>0</v>
-      </c>
-      <c r="CM6" t="n">
-        <v>0</v>
-      </c>
-      <c r="CN6" t="n">
-        <v>0</v>
-      </c>
-      <c r="CO6" t="n">
-        <v>0</v>
-      </c>
-      <c r="CP6" t="n">
-        <v>0</v>
-      </c>
-      <c r="CQ6" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR6" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS6" t="n">
-        <v>0</v>
-      </c>
-      <c r="CT6" t="n">
-        <v>0</v>
-      </c>
-      <c r="CU6" t="n">
-        <v>0</v>
-      </c>
-      <c r="CV6" t="n">
-        <v>0</v>
-      </c>
-      <c r="CW6" t="n">
-        <v>0</v>
-      </c>
       <c r="CX6" t="n">
         <v>0</v>
       </c>
@@ -2597,6 +2801,42 @@
         <v>0</v>
       </c>
       <c r="DH6" t="n">
+        <v>0</v>
+      </c>
+      <c r="DI6" t="n">
+        <v>0</v>
+      </c>
+      <c r="DJ6" t="n">
+        <v>0</v>
+      </c>
+      <c r="DK6" t="n">
+        <v>0</v>
+      </c>
+      <c r="DL6" t="n">
+        <v>0</v>
+      </c>
+      <c r="DM6" t="n">
+        <v>0</v>
+      </c>
+      <c r="DN6" t="n">
+        <v>0</v>
+      </c>
+      <c r="DO6" t="n">
+        <v>0</v>
+      </c>
+      <c r="DP6" t="n">
+        <v>0</v>
+      </c>
+      <c r="DQ6" t="n">
+        <v>0</v>
+      </c>
+      <c r="DR6" t="n">
+        <v>0</v>
+      </c>
+      <c r="DS6" t="n">
+        <v>0</v>
+      </c>
+      <c r="DT6" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2667,7 +2907,7 @@
       <c r="Z7" t="inlineStr"/>
       <c r="AA7" t="inlineStr"/>
       <c r="AB7" s="2" t="n">
-        <v>44313</v>
+        <v>44420</v>
       </c>
       <c r="AC7" t="n">
         <v>0</v>
@@ -2730,16 +2970,16 @@
         <v>0</v>
       </c>
       <c r="AW7" t="n">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="AX7" t="n">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="AY7" t="n">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="AZ7" t="n">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="BA7" t="n">
         <v>0</v>
@@ -2790,16 +3030,16 @@
         <v>0</v>
       </c>
       <c r="BQ7" t="n">
-        <v>2500</v>
+        <v>0</v>
       </c>
       <c r="BR7" t="n">
-        <v>2500</v>
+        <v>0</v>
       </c>
       <c r="BS7" t="n">
-        <v>2500</v>
+        <v>0</v>
       </c>
       <c r="BT7" t="n">
-        <v>2500</v>
+        <v>0</v>
       </c>
       <c r="BU7" t="n">
         <v>0</v>
@@ -2826,68 +3066,68 @@
         <v>0</v>
       </c>
       <c r="CC7" t="n">
+        <v>0</v>
+      </c>
+      <c r="CD7" t="n">
+        <v>0</v>
+      </c>
+      <c r="CE7" t="n">
+        <v>0</v>
+      </c>
+      <c r="CF7" t="n">
+        <v>0</v>
+      </c>
+      <c r="CG7" t="n">
+        <v>0</v>
+      </c>
+      <c r="CH7" t="n">
+        <v>0</v>
+      </c>
+      <c r="CI7" t="n">
+        <v>0</v>
+      </c>
+      <c r="CJ7" t="n">
+        <v>0</v>
+      </c>
+      <c r="CK7" t="n">
+        <v>0</v>
+      </c>
+      <c r="CL7" t="n">
+        <v>0</v>
+      </c>
+      <c r="CM7" t="n">
+        <v>0</v>
+      </c>
+      <c r="CN7" t="n">
+        <v>0</v>
+      </c>
+      <c r="CO7" t="n">
+        <v>0</v>
+      </c>
+      <c r="CP7" t="n">
+        <v>0</v>
+      </c>
+      <c r="CQ7" t="n">
+        <v>0</v>
+      </c>
+      <c r="CR7" t="n">
+        <v>0</v>
+      </c>
+      <c r="CS7" t="n">
+        <v>0</v>
+      </c>
+      <c r="CT7" t="n">
+        <v>0</v>
+      </c>
+      <c r="CU7" t="n">
+        <v>0</v>
+      </c>
+      <c r="CV7" t="n">
+        <v>0</v>
+      </c>
+      <c r="CW7" t="n">
         <v>100</v>
       </c>
-      <c r="CD7" t="n">
-        <v>0</v>
-      </c>
-      <c r="CE7" t="n">
-        <v>0</v>
-      </c>
-      <c r="CF7" t="n">
-        <v>0</v>
-      </c>
-      <c r="CG7" t="n">
-        <v>0</v>
-      </c>
-      <c r="CH7" t="n">
-        <v>0</v>
-      </c>
-      <c r="CI7" t="n">
-        <v>0</v>
-      </c>
-      <c r="CJ7" t="n">
-        <v>0</v>
-      </c>
-      <c r="CK7" t="n">
-        <v>0</v>
-      </c>
-      <c r="CL7" t="n">
-        <v>0</v>
-      </c>
-      <c r="CM7" t="n">
-        <v>0</v>
-      </c>
-      <c r="CN7" t="n">
-        <v>0</v>
-      </c>
-      <c r="CO7" t="n">
-        <v>0</v>
-      </c>
-      <c r="CP7" t="n">
-        <v>0</v>
-      </c>
-      <c r="CQ7" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR7" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS7" t="n">
-        <v>0</v>
-      </c>
-      <c r="CT7" t="n">
-        <v>0</v>
-      </c>
-      <c r="CU7" t="n">
-        <v>0</v>
-      </c>
-      <c r="CV7" t="n">
-        <v>0</v>
-      </c>
-      <c r="CW7" t="n">
-        <v>0</v>
-      </c>
       <c r="CX7" t="n">
         <v>0</v>
       </c>
@@ -2919,6 +3159,42 @@
         <v>0</v>
       </c>
       <c r="DH7" t="n">
+        <v>0</v>
+      </c>
+      <c r="DI7" t="n">
+        <v>0</v>
+      </c>
+      <c r="DJ7" t="n">
+        <v>0</v>
+      </c>
+      <c r="DK7" t="n">
+        <v>0</v>
+      </c>
+      <c r="DL7" t="n">
+        <v>0</v>
+      </c>
+      <c r="DM7" t="n">
+        <v>0</v>
+      </c>
+      <c r="DN7" t="n">
+        <v>0</v>
+      </c>
+      <c r="DO7" t="n">
+        <v>0</v>
+      </c>
+      <c r="DP7" t="n">
+        <v>0</v>
+      </c>
+      <c r="DQ7" t="n">
+        <v>0</v>
+      </c>
+      <c r="DR7" t="n">
+        <v>0</v>
+      </c>
+      <c r="DS7" t="n">
+        <v>0</v>
+      </c>
+      <c r="DT7" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2989,7 +3265,7 @@
       <c r="Z8" t="inlineStr"/>
       <c r="AA8" t="inlineStr"/>
       <c r="AB8" s="2" t="n">
-        <v>44313</v>
+        <v>44420</v>
       </c>
       <c r="AC8" t="n">
         <v>0</v>
@@ -3052,16 +3328,16 @@
         <v>0</v>
       </c>
       <c r="AW8" t="n">
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="AX8" t="n">
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="AY8" t="n">
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="AZ8" t="n">
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="BA8" t="n">
         <v>0</v>
@@ -3112,16 +3388,16 @@
         <v>0</v>
       </c>
       <c r="BQ8" t="n">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="BR8" t="n">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="BS8" t="n">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="BT8" t="n">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="BU8" t="n">
         <v>0</v>
@@ -3148,68 +3424,68 @@
         <v>0</v>
       </c>
       <c r="CC8" t="n">
+        <v>0</v>
+      </c>
+      <c r="CD8" t="n">
+        <v>0</v>
+      </c>
+      <c r="CE8" t="n">
+        <v>0</v>
+      </c>
+      <c r="CF8" t="n">
+        <v>0</v>
+      </c>
+      <c r="CG8" t="n">
+        <v>0</v>
+      </c>
+      <c r="CH8" t="n">
+        <v>0</v>
+      </c>
+      <c r="CI8" t="n">
+        <v>0</v>
+      </c>
+      <c r="CJ8" t="n">
+        <v>0</v>
+      </c>
+      <c r="CK8" t="n">
+        <v>0</v>
+      </c>
+      <c r="CL8" t="n">
+        <v>0</v>
+      </c>
+      <c r="CM8" t="n">
+        <v>0</v>
+      </c>
+      <c r="CN8" t="n">
+        <v>0</v>
+      </c>
+      <c r="CO8" t="n">
+        <v>0</v>
+      </c>
+      <c r="CP8" t="n">
+        <v>0</v>
+      </c>
+      <c r="CQ8" t="n">
+        <v>0</v>
+      </c>
+      <c r="CR8" t="n">
+        <v>0</v>
+      </c>
+      <c r="CS8" t="n">
+        <v>0</v>
+      </c>
+      <c r="CT8" t="n">
+        <v>0</v>
+      </c>
+      <c r="CU8" t="n">
+        <v>0</v>
+      </c>
+      <c r="CV8" t="n">
+        <v>0</v>
+      </c>
+      <c r="CW8" t="n">
         <v>200</v>
       </c>
-      <c r="CD8" t="n">
-        <v>0</v>
-      </c>
-      <c r="CE8" t="n">
-        <v>0</v>
-      </c>
-      <c r="CF8" t="n">
-        <v>0</v>
-      </c>
-      <c r="CG8" t="n">
-        <v>0</v>
-      </c>
-      <c r="CH8" t="n">
-        <v>0</v>
-      </c>
-      <c r="CI8" t="n">
-        <v>0</v>
-      </c>
-      <c r="CJ8" t="n">
-        <v>0</v>
-      </c>
-      <c r="CK8" t="n">
-        <v>0</v>
-      </c>
-      <c r="CL8" t="n">
-        <v>0</v>
-      </c>
-      <c r="CM8" t="n">
-        <v>0</v>
-      </c>
-      <c r="CN8" t="n">
-        <v>0</v>
-      </c>
-      <c r="CO8" t="n">
-        <v>0</v>
-      </c>
-      <c r="CP8" t="n">
-        <v>0</v>
-      </c>
-      <c r="CQ8" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR8" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS8" t="n">
-        <v>0</v>
-      </c>
-      <c r="CT8" t="n">
-        <v>0</v>
-      </c>
-      <c r="CU8" t="n">
-        <v>0</v>
-      </c>
-      <c r="CV8" t="n">
-        <v>0</v>
-      </c>
-      <c r="CW8" t="n">
-        <v>0</v>
-      </c>
       <c r="CX8" t="n">
         <v>0</v>
       </c>
@@ -3241,6 +3517,42 @@
         <v>0</v>
       </c>
       <c r="DH8" t="n">
+        <v>0</v>
+      </c>
+      <c r="DI8" t="n">
+        <v>0</v>
+      </c>
+      <c r="DJ8" t="n">
+        <v>0</v>
+      </c>
+      <c r="DK8" t="n">
+        <v>0</v>
+      </c>
+      <c r="DL8" t="n">
+        <v>0</v>
+      </c>
+      <c r="DM8" t="n">
+        <v>0</v>
+      </c>
+      <c r="DN8" t="n">
+        <v>0</v>
+      </c>
+      <c r="DO8" t="n">
+        <v>0</v>
+      </c>
+      <c r="DP8" t="n">
+        <v>0</v>
+      </c>
+      <c r="DQ8" t="n">
+        <v>0</v>
+      </c>
+      <c r="DR8" t="n">
+        <v>0</v>
+      </c>
+      <c r="DS8" t="n">
+        <v>0</v>
+      </c>
+      <c r="DT8" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3311,7 +3623,7 @@
       <c r="Z9" t="inlineStr"/>
       <c r="AA9" t="inlineStr"/>
       <c r="AB9" s="2" t="n">
-        <v>44313</v>
+        <v>44420</v>
       </c>
       <c r="AC9" t="n">
         <v>0</v>
@@ -3374,16 +3686,16 @@
         <v>0</v>
       </c>
       <c r="AW9" t="n">
-        <v>0</v>
+        <v>625</v>
       </c>
       <c r="AX9" t="n">
-        <v>0</v>
+        <v>625</v>
       </c>
       <c r="AY9" t="n">
-        <v>0</v>
+        <v>625</v>
       </c>
       <c r="AZ9" t="n">
-        <v>0</v>
+        <v>625</v>
       </c>
       <c r="BA9" t="n">
         <v>0</v>
@@ -3434,16 +3746,16 @@
         <v>0</v>
       </c>
       <c r="BQ9" t="n">
-        <v>625</v>
+        <v>0</v>
       </c>
       <c r="BR9" t="n">
-        <v>625</v>
+        <v>0</v>
       </c>
       <c r="BS9" t="n">
-        <v>625</v>
+        <v>0</v>
       </c>
       <c r="BT9" t="n">
-        <v>625</v>
+        <v>0</v>
       </c>
       <c r="BU9" t="n">
         <v>0</v>
@@ -3470,68 +3782,68 @@
         <v>0</v>
       </c>
       <c r="CC9" t="n">
+        <v>0</v>
+      </c>
+      <c r="CD9" t="n">
+        <v>0</v>
+      </c>
+      <c r="CE9" t="n">
+        <v>0</v>
+      </c>
+      <c r="CF9" t="n">
+        <v>0</v>
+      </c>
+      <c r="CG9" t="n">
+        <v>0</v>
+      </c>
+      <c r="CH9" t="n">
+        <v>0</v>
+      </c>
+      <c r="CI9" t="n">
+        <v>0</v>
+      </c>
+      <c r="CJ9" t="n">
+        <v>0</v>
+      </c>
+      <c r="CK9" t="n">
+        <v>0</v>
+      </c>
+      <c r="CL9" t="n">
+        <v>0</v>
+      </c>
+      <c r="CM9" t="n">
+        <v>0</v>
+      </c>
+      <c r="CN9" t="n">
+        <v>0</v>
+      </c>
+      <c r="CO9" t="n">
+        <v>0</v>
+      </c>
+      <c r="CP9" t="n">
+        <v>0</v>
+      </c>
+      <c r="CQ9" t="n">
+        <v>0</v>
+      </c>
+      <c r="CR9" t="n">
+        <v>0</v>
+      </c>
+      <c r="CS9" t="n">
+        <v>0</v>
+      </c>
+      <c r="CT9" t="n">
+        <v>0</v>
+      </c>
+      <c r="CU9" t="n">
+        <v>0</v>
+      </c>
+      <c r="CV9" t="n">
+        <v>0</v>
+      </c>
+      <c r="CW9" t="n">
         <v>700</v>
       </c>
-      <c r="CD9" t="n">
-        <v>0</v>
-      </c>
-      <c r="CE9" t="n">
-        <v>0</v>
-      </c>
-      <c r="CF9" t="n">
-        <v>0</v>
-      </c>
-      <c r="CG9" t="n">
-        <v>0</v>
-      </c>
-      <c r="CH9" t="n">
-        <v>0</v>
-      </c>
-      <c r="CI9" t="n">
-        <v>0</v>
-      </c>
-      <c r="CJ9" t="n">
-        <v>0</v>
-      </c>
-      <c r="CK9" t="n">
-        <v>0</v>
-      </c>
-      <c r="CL9" t="n">
-        <v>0</v>
-      </c>
-      <c r="CM9" t="n">
-        <v>0</v>
-      </c>
-      <c r="CN9" t="n">
-        <v>0</v>
-      </c>
-      <c r="CO9" t="n">
-        <v>0</v>
-      </c>
-      <c r="CP9" t="n">
-        <v>0</v>
-      </c>
-      <c r="CQ9" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR9" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS9" t="n">
-        <v>0</v>
-      </c>
-      <c r="CT9" t="n">
-        <v>0</v>
-      </c>
-      <c r="CU9" t="n">
-        <v>0</v>
-      </c>
-      <c r="CV9" t="n">
-        <v>0</v>
-      </c>
-      <c r="CW9" t="n">
-        <v>0</v>
-      </c>
       <c r="CX9" t="n">
         <v>0</v>
       </c>
@@ -3563,6 +3875,42 @@
         <v>0</v>
       </c>
       <c r="DH9" t="n">
+        <v>0</v>
+      </c>
+      <c r="DI9" t="n">
+        <v>0</v>
+      </c>
+      <c r="DJ9" t="n">
+        <v>0</v>
+      </c>
+      <c r="DK9" t="n">
+        <v>0</v>
+      </c>
+      <c r="DL9" t="n">
+        <v>0</v>
+      </c>
+      <c r="DM9" t="n">
+        <v>0</v>
+      </c>
+      <c r="DN9" t="n">
+        <v>0</v>
+      </c>
+      <c r="DO9" t="n">
+        <v>0</v>
+      </c>
+      <c r="DP9" t="n">
+        <v>0</v>
+      </c>
+      <c r="DQ9" t="n">
+        <v>0</v>
+      </c>
+      <c r="DR9" t="n">
+        <v>0</v>
+      </c>
+      <c r="DS9" t="n">
+        <v>0</v>
+      </c>
+      <c r="DT9" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3633,7 +3981,7 @@
       <c r="Z10" t="inlineStr"/>
       <c r="AA10" t="inlineStr"/>
       <c r="AB10" s="2" t="n">
-        <v>44313</v>
+        <v>44420</v>
       </c>
       <c r="AC10" t="n">
         <v>0</v>
@@ -3696,16 +4044,16 @@
         <v>0</v>
       </c>
       <c r="AW10" t="n">
-        <v>0</v>
+        <v>375</v>
       </c>
       <c r="AX10" t="n">
-        <v>0</v>
+        <v>375</v>
       </c>
       <c r="AY10" t="n">
-        <v>0</v>
+        <v>375</v>
       </c>
       <c r="AZ10" t="n">
-        <v>0</v>
+        <v>375</v>
       </c>
       <c r="BA10" t="n">
         <v>0</v>
@@ -3756,16 +4104,16 @@
         <v>0</v>
       </c>
       <c r="BQ10" t="n">
-        <v>375</v>
+        <v>0</v>
       </c>
       <c r="BR10" t="n">
-        <v>375</v>
+        <v>0</v>
       </c>
       <c r="BS10" t="n">
-        <v>375</v>
+        <v>0</v>
       </c>
       <c r="BT10" t="n">
-        <v>375</v>
+        <v>0</v>
       </c>
       <c r="BU10" t="n">
         <v>0</v>
@@ -3792,68 +4140,68 @@
         <v>0</v>
       </c>
       <c r="CC10" t="n">
+        <v>0</v>
+      </c>
+      <c r="CD10" t="n">
+        <v>0</v>
+      </c>
+      <c r="CE10" t="n">
+        <v>0</v>
+      </c>
+      <c r="CF10" t="n">
+        <v>0</v>
+      </c>
+      <c r="CG10" t="n">
+        <v>0</v>
+      </c>
+      <c r="CH10" t="n">
+        <v>0</v>
+      </c>
+      <c r="CI10" t="n">
+        <v>0</v>
+      </c>
+      <c r="CJ10" t="n">
+        <v>0</v>
+      </c>
+      <c r="CK10" t="n">
+        <v>0</v>
+      </c>
+      <c r="CL10" t="n">
+        <v>0</v>
+      </c>
+      <c r="CM10" t="n">
+        <v>0</v>
+      </c>
+      <c r="CN10" t="n">
+        <v>0</v>
+      </c>
+      <c r="CO10" t="n">
+        <v>0</v>
+      </c>
+      <c r="CP10" t="n">
+        <v>0</v>
+      </c>
+      <c r="CQ10" t="n">
+        <v>0</v>
+      </c>
+      <c r="CR10" t="n">
+        <v>0</v>
+      </c>
+      <c r="CS10" t="n">
+        <v>0</v>
+      </c>
+      <c r="CT10" t="n">
+        <v>0</v>
+      </c>
+      <c r="CU10" t="n">
+        <v>0</v>
+      </c>
+      <c r="CV10" t="n">
+        <v>0</v>
+      </c>
+      <c r="CW10" t="n">
         <v>450</v>
       </c>
-      <c r="CD10" t="n">
-        <v>0</v>
-      </c>
-      <c r="CE10" t="n">
-        <v>0</v>
-      </c>
-      <c r="CF10" t="n">
-        <v>0</v>
-      </c>
-      <c r="CG10" t="n">
-        <v>0</v>
-      </c>
-      <c r="CH10" t="n">
-        <v>0</v>
-      </c>
-      <c r="CI10" t="n">
-        <v>0</v>
-      </c>
-      <c r="CJ10" t="n">
-        <v>0</v>
-      </c>
-      <c r="CK10" t="n">
-        <v>0</v>
-      </c>
-      <c r="CL10" t="n">
-        <v>0</v>
-      </c>
-      <c r="CM10" t="n">
-        <v>0</v>
-      </c>
-      <c r="CN10" t="n">
-        <v>0</v>
-      </c>
-      <c r="CO10" t="n">
-        <v>0</v>
-      </c>
-      <c r="CP10" t="n">
-        <v>0</v>
-      </c>
-      <c r="CQ10" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR10" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS10" t="n">
-        <v>0</v>
-      </c>
-      <c r="CT10" t="n">
-        <v>0</v>
-      </c>
-      <c r="CU10" t="n">
-        <v>0</v>
-      </c>
-      <c r="CV10" t="n">
-        <v>0</v>
-      </c>
-      <c r="CW10" t="n">
-        <v>0</v>
-      </c>
       <c r="CX10" t="n">
         <v>0</v>
       </c>
@@ -3885,6 +4233,42 @@
         <v>0</v>
       </c>
       <c r="DH10" t="n">
+        <v>0</v>
+      </c>
+      <c r="DI10" t="n">
+        <v>0</v>
+      </c>
+      <c r="DJ10" t="n">
+        <v>0</v>
+      </c>
+      <c r="DK10" t="n">
+        <v>0</v>
+      </c>
+      <c r="DL10" t="n">
+        <v>0</v>
+      </c>
+      <c r="DM10" t="n">
+        <v>0</v>
+      </c>
+      <c r="DN10" t="n">
+        <v>0</v>
+      </c>
+      <c r="DO10" t="n">
+        <v>0</v>
+      </c>
+      <c r="DP10" t="n">
+        <v>0</v>
+      </c>
+      <c r="DQ10" t="n">
+        <v>0</v>
+      </c>
+      <c r="DR10" t="n">
+        <v>0</v>
+      </c>
+      <c r="DS10" t="n">
+        <v>0</v>
+      </c>
+      <c r="DT10" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3955,7 +4339,7 @@
       <c r="Z11" t="inlineStr"/>
       <c r="AA11" t="inlineStr"/>
       <c r="AB11" s="2" t="n">
-        <v>44313</v>
+        <v>44420</v>
       </c>
       <c r="AC11" t="n">
         <v>0</v>
@@ -4018,16 +4402,16 @@
         <v>0</v>
       </c>
       <c r="AW11" t="n">
-        <v>0</v>
+        <v>750</v>
       </c>
       <c r="AX11" t="n">
-        <v>0</v>
+        <v>750</v>
       </c>
       <c r="AY11" t="n">
-        <v>0</v>
+        <v>750</v>
       </c>
       <c r="AZ11" t="n">
-        <v>0</v>
+        <v>750</v>
       </c>
       <c r="BA11" t="n">
         <v>0</v>
@@ -4078,16 +4462,16 @@
         <v>0</v>
       </c>
       <c r="BQ11" t="n">
-        <v>750</v>
+        <v>0</v>
       </c>
       <c r="BR11" t="n">
-        <v>750</v>
+        <v>0</v>
       </c>
       <c r="BS11" t="n">
-        <v>750</v>
+        <v>0</v>
       </c>
       <c r="BT11" t="n">
-        <v>750</v>
+        <v>0</v>
       </c>
       <c r="BU11" t="n">
         <v>0</v>
@@ -4114,68 +4498,68 @@
         <v>0</v>
       </c>
       <c r="CC11" t="n">
+        <v>0</v>
+      </c>
+      <c r="CD11" t="n">
+        <v>0</v>
+      </c>
+      <c r="CE11" t="n">
+        <v>0</v>
+      </c>
+      <c r="CF11" t="n">
+        <v>0</v>
+      </c>
+      <c r="CG11" t="n">
+        <v>0</v>
+      </c>
+      <c r="CH11" t="n">
+        <v>0</v>
+      </c>
+      <c r="CI11" t="n">
+        <v>0</v>
+      </c>
+      <c r="CJ11" t="n">
+        <v>0</v>
+      </c>
+      <c r="CK11" t="n">
+        <v>0</v>
+      </c>
+      <c r="CL11" t="n">
+        <v>0</v>
+      </c>
+      <c r="CM11" t="n">
+        <v>0</v>
+      </c>
+      <c r="CN11" t="n">
+        <v>0</v>
+      </c>
+      <c r="CO11" t="n">
+        <v>0</v>
+      </c>
+      <c r="CP11" t="n">
+        <v>0</v>
+      </c>
+      <c r="CQ11" t="n">
+        <v>0</v>
+      </c>
+      <c r="CR11" t="n">
+        <v>0</v>
+      </c>
+      <c r="CS11" t="n">
+        <v>0</v>
+      </c>
+      <c r="CT11" t="n">
+        <v>0</v>
+      </c>
+      <c r="CU11" t="n">
+        <v>0</v>
+      </c>
+      <c r="CV11" t="n">
+        <v>0</v>
+      </c>
+      <c r="CW11" t="n">
         <v>1300</v>
       </c>
-      <c r="CD11" t="n">
-        <v>0</v>
-      </c>
-      <c r="CE11" t="n">
-        <v>0</v>
-      </c>
-      <c r="CF11" t="n">
-        <v>0</v>
-      </c>
-      <c r="CG11" t="n">
-        <v>0</v>
-      </c>
-      <c r="CH11" t="n">
-        <v>0</v>
-      </c>
-      <c r="CI11" t="n">
-        <v>0</v>
-      </c>
-      <c r="CJ11" t="n">
-        <v>0</v>
-      </c>
-      <c r="CK11" t="n">
-        <v>0</v>
-      </c>
-      <c r="CL11" t="n">
-        <v>0</v>
-      </c>
-      <c r="CM11" t="n">
-        <v>0</v>
-      </c>
-      <c r="CN11" t="n">
-        <v>0</v>
-      </c>
-      <c r="CO11" t="n">
-        <v>0</v>
-      </c>
-      <c r="CP11" t="n">
-        <v>0</v>
-      </c>
-      <c r="CQ11" t="n">
-        <v>0</v>
-      </c>
-      <c r="CR11" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS11" t="n">
-        <v>0</v>
-      </c>
-      <c r="CT11" t="n">
-        <v>0</v>
-      </c>
-      <c r="CU11" t="n">
-        <v>0</v>
-      </c>
-      <c r="CV11" t="n">
-        <v>0</v>
-      </c>
-      <c r="CW11" t="n">
-        <v>0</v>
-      </c>
       <c r="CX11" t="n">
         <v>0</v>
       </c>
@@ -4207,6 +4591,42 @@
         <v>0</v>
       </c>
       <c r="DH11" t="n">
+        <v>0</v>
+      </c>
+      <c r="DI11" t="n">
+        <v>0</v>
+      </c>
+      <c r="DJ11" t="n">
+        <v>0</v>
+      </c>
+      <c r="DK11" t="n">
+        <v>0</v>
+      </c>
+      <c r="DL11" t="n">
+        <v>0</v>
+      </c>
+      <c r="DM11" t="n">
+        <v>0</v>
+      </c>
+      <c r="DN11" t="n">
+        <v>0</v>
+      </c>
+      <c r="DO11" t="n">
+        <v>0</v>
+      </c>
+      <c r="DP11" t="n">
+        <v>0</v>
+      </c>
+      <c r="DQ11" t="n">
+        <v>0</v>
+      </c>
+      <c r="DR11" t="n">
+        <v>0</v>
+      </c>
+      <c r="DS11" t="n">
+        <v>0</v>
+      </c>
+      <c r="DT11" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update artefacts to reflect added SDG Goal column to exports
</commit_message>
<xml_diff>
--- a/tests/artefacts/api/exports/activities_xlsx.xlsx
+++ b/tests/artefacts/api/exports/activities_xlsx.xlsx
@@ -420,7 +420,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:EC11"/>
+  <dimension ref="A1:ED11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -521,575 +521,580 @@
       </c>
       <c r="S1" s="1" t="inlineStr">
         <is>
+          <t>SDG Goal</t>
+        </is>
+      </c>
+      <c r="T1" s="1" t="inlineStr">
+        <is>
           <t>Collaboration Type (Donor Type)</t>
         </is>
       </c>
-      <c r="T1" s="1" t="inlineStr">
+      <c r="U1" s="1" t="inlineStr">
         <is>
           <t>Fund Source</t>
         </is>
       </c>
-      <c r="U1" s="1" t="inlineStr">
+      <c r="V1" s="1" t="inlineStr">
         <is>
           <t>Finance Type (Type of Assistance)</t>
         </is>
       </c>
-      <c r="V1" s="1" t="inlineStr">
+      <c r="W1" s="1" t="inlineStr">
         <is>
           <t>Aid Type (Aid Modality)</t>
         </is>
       </c>
-      <c r="W1" s="1" t="inlineStr">
+      <c r="X1" s="1" t="inlineStr">
         <is>
           <t>Activity Budget</t>
         </is>
       </c>
-      <c r="X1" s="1" t="inlineStr">
+      <c r="Y1" s="1" t="inlineStr">
         <is>
           <t>Planned Disbursements</t>
         </is>
       </c>
-      <c r="Y1" s="1" t="inlineStr">
+      <c r="Z1" s="1" t="inlineStr">
         <is>
           <t>Total Commitments</t>
         </is>
       </c>
-      <c r="Z1" s="1" t="inlineStr">
+      <c r="AA1" s="1" t="inlineStr">
         <is>
           <t>Total Disbursements</t>
         </is>
       </c>
-      <c r="AA1" s="1" t="inlineStr">
+      <c r="AB1" s="1" t="inlineStr">
         <is>
           <t>Activity Documents</t>
         </is>
       </c>
-      <c r="AB1" s="1" t="inlineStr">
+      <c r="AC1" s="1" t="inlineStr">
         <is>
           <t>Activity Website</t>
         </is>
       </c>
-      <c r="AC1" s="1" t="inlineStr">
+      <c r="AD1" s="1" t="inlineStr">
         <is>
           <t>Last updated date</t>
         </is>
       </c>
-      <c r="AD1" s="1" t="inlineStr">
+      <c r="AE1" s="1" t="inlineStr">
         <is>
           <t>FY2013 Q1 (MTEF)</t>
         </is>
       </c>
-      <c r="AE1" s="1" t="inlineStr">
+      <c r="AF1" s="1" t="inlineStr">
         <is>
           <t>FY2013 Q2 (MTEF)</t>
         </is>
       </c>
-      <c r="AF1" s="1" t="inlineStr">
+      <c r="AG1" s="1" t="inlineStr">
         <is>
           <t>FY2013 Q3 (MTEF)</t>
         </is>
       </c>
-      <c r="AG1" s="1" t="inlineStr">
+      <c r="AH1" s="1" t="inlineStr">
         <is>
           <t>FY2013 Q4 (MTEF)</t>
         </is>
       </c>
-      <c r="AH1" s="1" t="inlineStr">
+      <c r="AI1" s="1" t="inlineStr">
         <is>
           <t>FY2014 Q1 (MTEF)</t>
         </is>
       </c>
-      <c r="AI1" s="1" t="inlineStr">
+      <c r="AJ1" s="1" t="inlineStr">
         <is>
           <t>FY2014 Q2 (MTEF)</t>
         </is>
       </c>
-      <c r="AJ1" s="1" t="inlineStr">
+      <c r="AK1" s="1" t="inlineStr">
         <is>
           <t>FY2014 Q3 (MTEF)</t>
         </is>
       </c>
-      <c r="AK1" s="1" t="inlineStr">
+      <c r="AL1" s="1" t="inlineStr">
         <is>
           <t>FY2014 Q4 (MTEF)</t>
         </is>
       </c>
-      <c r="AL1" s="1" t="inlineStr">
+      <c r="AM1" s="1" t="inlineStr">
         <is>
           <t>FY2015 Q1 (MTEF)</t>
         </is>
       </c>
-      <c r="AM1" s="1" t="inlineStr">
+      <c r="AN1" s="1" t="inlineStr">
         <is>
           <t>FY2015 Q2 (MTEF)</t>
         </is>
       </c>
-      <c r="AN1" s="1" t="inlineStr">
+      <c r="AO1" s="1" t="inlineStr">
         <is>
           <t>FY2015 Q3 (MTEF)</t>
         </is>
       </c>
-      <c r="AO1" s="1" t="inlineStr">
+      <c r="AP1" s="1" t="inlineStr">
         <is>
           <t>FY2015 Q4 (MTEF)</t>
         </is>
       </c>
-      <c r="AP1" s="1" t="inlineStr">
+      <c r="AQ1" s="1" t="inlineStr">
         <is>
           <t>FY2016 Q1 (MTEF)</t>
         </is>
       </c>
-      <c r="AQ1" s="1" t="inlineStr">
+      <c r="AR1" s="1" t="inlineStr">
         <is>
           <t>FY2016 Q2 (MTEF)</t>
         </is>
       </c>
-      <c r="AR1" s="1" t="inlineStr">
+      <c r="AS1" s="1" t="inlineStr">
         <is>
           <t>FY2016 Q3 (MTEF)</t>
         </is>
       </c>
-      <c r="AS1" s="1" t="inlineStr">
+      <c r="AT1" s="1" t="inlineStr">
         <is>
           <t>FY2016 Q4 (MTEF)</t>
         </is>
       </c>
-      <c r="AT1" s="1" t="inlineStr">
+      <c r="AU1" s="1" t="inlineStr">
         <is>
           <t>FY2017 Q1 (MTEF)</t>
         </is>
       </c>
-      <c r="AU1" s="1" t="inlineStr">
+      <c r="AV1" s="1" t="inlineStr">
         <is>
           <t>FY2017 Q2 (MTEF)</t>
         </is>
       </c>
-      <c r="AV1" s="1" t="inlineStr">
+      <c r="AW1" s="1" t="inlineStr">
         <is>
           <t>FY2017 Q3 (MTEF)</t>
         </is>
       </c>
-      <c r="AW1" s="1" t="inlineStr">
+      <c r="AX1" s="1" t="inlineStr">
         <is>
           <t>FY2017 Q4 (MTEF)</t>
         </is>
       </c>
-      <c r="AX1" s="1" t="inlineStr">
+      <c r="AY1" s="1" t="inlineStr">
         <is>
           <t>FY2018 Q1 (MTEF)</t>
         </is>
       </c>
-      <c r="AY1" s="1" t="inlineStr">
+      <c r="AZ1" s="1" t="inlineStr">
         <is>
           <t>FY2018 Q2 (MTEF)</t>
         </is>
       </c>
-      <c r="AZ1" s="1" t="inlineStr">
+      <c r="BA1" s="1" t="inlineStr">
         <is>
           <t>FY2018 Q3 (MTEF)</t>
         </is>
       </c>
-      <c r="BA1" s="1" t="inlineStr">
+      <c r="BB1" s="1" t="inlineStr">
         <is>
           <t>FY2018 Q4 (MTEF)</t>
         </is>
       </c>
-      <c r="BB1" s="1" t="inlineStr">
+      <c r="BC1" s="1" t="inlineStr">
         <is>
           <t>FY2019 Q1 (MTEF)</t>
         </is>
       </c>
-      <c r="BC1" s="1" t="inlineStr">
+      <c r="BD1" s="1" t="inlineStr">
         <is>
           <t>FY2019 Q2 (MTEF)</t>
         </is>
       </c>
-      <c r="BD1" s="1" t="inlineStr">
+      <c r="BE1" s="1" t="inlineStr">
         <is>
           <t>FY2019 Q3 (MTEF)</t>
         </is>
       </c>
-      <c r="BE1" s="1" t="inlineStr">
+      <c r="BF1" s="1" t="inlineStr">
         <is>
           <t>FY2019 Q4 (MTEF)</t>
         </is>
       </c>
-      <c r="BF1" s="1" t="inlineStr">
+      <c r="BG1" s="1" t="inlineStr">
         <is>
           <t>FY2020 Q1 (MTEF)</t>
         </is>
       </c>
-      <c r="BG1" s="1" t="inlineStr">
+      <c r="BH1" s="1" t="inlineStr">
         <is>
           <t>FY2020 Q2 (MTEF)</t>
         </is>
       </c>
-      <c r="BH1" s="1" t="inlineStr">
+      <c r="BI1" s="1" t="inlineStr">
         <is>
           <t>FY2020 Q3 (MTEF)</t>
         </is>
       </c>
-      <c r="BI1" s="1" t="inlineStr">
+      <c r="BJ1" s="1" t="inlineStr">
         <is>
           <t>FY2020 Q4 (MTEF)</t>
         </is>
       </c>
-      <c r="BJ1" s="1" t="inlineStr">
+      <c r="BK1" s="1" t="inlineStr">
         <is>
           <t>FY2021 Q1 (MTEF)</t>
         </is>
       </c>
-      <c r="BK1" s="1" t="inlineStr">
+      <c r="BL1" s="1" t="inlineStr">
         <is>
           <t>FY2021 Q2 (MTEF)</t>
         </is>
       </c>
-      <c r="BL1" s="1" t="inlineStr">
+      <c r="BM1" s="1" t="inlineStr">
         <is>
           <t>FY2021 Q3 (MTEF)</t>
         </is>
       </c>
-      <c r="BM1" s="1" t="inlineStr">
+      <c r="BN1" s="1" t="inlineStr">
         <is>
           <t>FY2021 Q4 (MTEF)</t>
         </is>
       </c>
-      <c r="BN1" s="1" t="inlineStr">
+      <c r="BO1" s="1" t="inlineStr">
         <is>
           <t>FY2022 Q1 (MTEF)</t>
         </is>
       </c>
-      <c r="BO1" s="1" t="inlineStr">
+      <c r="BP1" s="1" t="inlineStr">
         <is>
           <t>FY2022 Q2 (MTEF)</t>
         </is>
       </c>
-      <c r="BP1" s="1" t="inlineStr">
+      <c r="BQ1" s="1" t="inlineStr">
         <is>
           <t>FY2022 Q3 (MTEF)</t>
         </is>
       </c>
-      <c r="BQ1" s="1" t="inlineStr">
+      <c r="BR1" s="1" t="inlineStr">
         <is>
           <t>FY2022 Q4 (MTEF)</t>
         </is>
       </c>
-      <c r="BR1" s="1" t="inlineStr">
+      <c r="BS1" s="1" t="inlineStr">
         <is>
           <t>FY2023 Q1 (MTEF)</t>
         </is>
       </c>
-      <c r="BS1" s="1" t="inlineStr">
+      <c r="BT1" s="1" t="inlineStr">
         <is>
           <t>FY2023 Q2 (MTEF)</t>
         </is>
       </c>
-      <c r="BT1" s="1" t="inlineStr">
+      <c r="BU1" s="1" t="inlineStr">
         <is>
           <t>FY2023 Q3 (MTEF)</t>
         </is>
       </c>
-      <c r="BU1" s="1" t="inlineStr">
+      <c r="BV1" s="1" t="inlineStr">
         <is>
           <t>FY2023 Q4 (MTEF)</t>
         </is>
       </c>
-      <c r="BV1" s="1" t="inlineStr">
+      <c r="BW1" s="1" t="inlineStr">
         <is>
           <t>FY2024 Q1 (MTEF)</t>
         </is>
       </c>
-      <c r="BW1" s="1" t="inlineStr">
+      <c r="BX1" s="1" t="inlineStr">
         <is>
           <t>FY2024 Q2 (MTEF)</t>
         </is>
       </c>
-      <c r="BX1" s="1" t="inlineStr">
+      <c r="BY1" s="1" t="inlineStr">
         <is>
           <t>FY2024 Q3 (MTEF)</t>
         </is>
       </c>
-      <c r="BY1" s="1" t="inlineStr">
+      <c r="BZ1" s="1" t="inlineStr">
         <is>
           <t>FY2024 Q4 (MTEF)</t>
         </is>
       </c>
-      <c r="BZ1" s="1" t="inlineStr">
+      <c r="CA1" s="1" t="inlineStr">
         <is>
           <t>FY2025 Q1 (MTEF)</t>
         </is>
       </c>
-      <c r="CA1" s="1" t="inlineStr">
+      <c r="CB1" s="1" t="inlineStr">
         <is>
           <t>FY2025 Q2 (MTEF)</t>
         </is>
       </c>
-      <c r="CB1" s="1" t="inlineStr">
+      <c r="CC1" s="1" t="inlineStr">
         <is>
           <t>FY2025 Q3 (MTEF)</t>
         </is>
       </c>
-      <c r="CC1" s="1" t="inlineStr">
+      <c r="CD1" s="1" t="inlineStr">
         <is>
           <t>FY2025 Q4 (MTEF)</t>
         </is>
       </c>
-      <c r="CD1" s="1" t="inlineStr">
+      <c r="CE1" s="1" t="inlineStr">
         <is>
           <t>FY2013 Q1 (D)</t>
         </is>
       </c>
-      <c r="CE1" s="1" t="inlineStr">
+      <c r="CF1" s="1" t="inlineStr">
         <is>
           <t>FY2013 Q2 (D)</t>
         </is>
       </c>
-      <c r="CF1" s="1" t="inlineStr">
+      <c r="CG1" s="1" t="inlineStr">
         <is>
           <t>FY2013 Q3 (D)</t>
         </is>
       </c>
-      <c r="CG1" s="1" t="inlineStr">
+      <c r="CH1" s="1" t="inlineStr">
         <is>
           <t>FY2013 Q4 (D)</t>
         </is>
       </c>
-      <c r="CH1" s="1" t="inlineStr">
+      <c r="CI1" s="1" t="inlineStr">
         <is>
           <t>FY2014 Q1 (D)</t>
         </is>
       </c>
-      <c r="CI1" s="1" t="inlineStr">
+      <c r="CJ1" s="1" t="inlineStr">
         <is>
           <t>FY2014 Q2 (D)</t>
         </is>
       </c>
-      <c r="CJ1" s="1" t="inlineStr">
+      <c r="CK1" s="1" t="inlineStr">
         <is>
           <t>FY2014 Q3 (D)</t>
         </is>
       </c>
-      <c r="CK1" s="1" t="inlineStr">
+      <c r="CL1" s="1" t="inlineStr">
         <is>
           <t>FY2014 Q4 (D)</t>
         </is>
       </c>
-      <c r="CL1" s="1" t="inlineStr">
+      <c r="CM1" s="1" t="inlineStr">
         <is>
           <t>FY2015 Q1 (D)</t>
         </is>
       </c>
-      <c r="CM1" s="1" t="inlineStr">
+      <c r="CN1" s="1" t="inlineStr">
         <is>
           <t>FY2015 Q2 (D)</t>
         </is>
       </c>
-      <c r="CN1" s="1" t="inlineStr">
+      <c r="CO1" s="1" t="inlineStr">
         <is>
           <t>FY2015 Q3 (D)</t>
         </is>
       </c>
-      <c r="CO1" s="1" t="inlineStr">
+      <c r="CP1" s="1" t="inlineStr">
         <is>
           <t>FY2015 Q4 (D)</t>
         </is>
       </c>
-      <c r="CP1" s="1" t="inlineStr">
+      <c r="CQ1" s="1" t="inlineStr">
         <is>
           <t>FY2016 Q1 (D)</t>
         </is>
       </c>
-      <c r="CQ1" s="1" t="inlineStr">
+      <c r="CR1" s="1" t="inlineStr">
         <is>
           <t>FY2016 Q2 (D)</t>
         </is>
       </c>
-      <c r="CR1" s="1" t="inlineStr">
+      <c r="CS1" s="1" t="inlineStr">
         <is>
           <t>FY2016 Q3 (D)</t>
         </is>
       </c>
-      <c r="CS1" s="1" t="inlineStr">
+      <c r="CT1" s="1" t="inlineStr">
         <is>
           <t>FY2016 Q4 (D)</t>
         </is>
       </c>
-      <c r="CT1" s="1" t="inlineStr">
+      <c r="CU1" s="1" t="inlineStr">
         <is>
           <t>FY2017 Q1 (D)</t>
         </is>
       </c>
-      <c r="CU1" s="1" t="inlineStr">
+      <c r="CV1" s="1" t="inlineStr">
         <is>
           <t>FY2017 Q2 (D)</t>
         </is>
       </c>
-      <c r="CV1" s="1" t="inlineStr">
+      <c r="CW1" s="1" t="inlineStr">
         <is>
           <t>FY2017 Q3 (D)</t>
         </is>
       </c>
-      <c r="CW1" s="1" t="inlineStr">
+      <c r="CX1" s="1" t="inlineStr">
         <is>
           <t>FY2017 Q4 (D)</t>
         </is>
       </c>
-      <c r="CX1" s="1" t="inlineStr">
+      <c r="CY1" s="1" t="inlineStr">
         <is>
           <t>FY2018 Q1 (D)</t>
         </is>
       </c>
-      <c r="CY1" s="1" t="inlineStr">
+      <c r="CZ1" s="1" t="inlineStr">
         <is>
           <t>FY2018 Q2 (D)</t>
         </is>
       </c>
-      <c r="CZ1" s="1" t="inlineStr">
+      <c r="DA1" s="1" t="inlineStr">
         <is>
           <t>FY2018 Q3 (D)</t>
         </is>
       </c>
-      <c r="DA1" s="1" t="inlineStr">
+      <c r="DB1" s="1" t="inlineStr">
         <is>
           <t>FY2018 Q4 (D)</t>
         </is>
       </c>
-      <c r="DB1" s="1" t="inlineStr">
+      <c r="DC1" s="1" t="inlineStr">
         <is>
           <t>FY2019 Q1 (D)</t>
         </is>
       </c>
-      <c r="DC1" s="1" t="inlineStr">
+      <c r="DD1" s="1" t="inlineStr">
         <is>
           <t>FY2019 Q2 (D)</t>
         </is>
       </c>
-      <c r="DD1" s="1" t="inlineStr">
+      <c r="DE1" s="1" t="inlineStr">
         <is>
           <t>FY2019 Q3 (D)</t>
         </is>
       </c>
-      <c r="DE1" s="1" t="inlineStr">
+      <c r="DF1" s="1" t="inlineStr">
         <is>
           <t>FY2019 Q4 (D)</t>
         </is>
       </c>
-      <c r="DF1" s="1" t="inlineStr">
+      <c r="DG1" s="1" t="inlineStr">
         <is>
           <t>FY2020 Q1 (D)</t>
         </is>
       </c>
-      <c r="DG1" s="1" t="inlineStr">
+      <c r="DH1" s="1" t="inlineStr">
         <is>
           <t>FY2020 Q2 (D)</t>
         </is>
       </c>
-      <c r="DH1" s="1" t="inlineStr">
+      <c r="DI1" s="1" t="inlineStr">
         <is>
           <t>FY2020 Q3 (D)</t>
         </is>
       </c>
-      <c r="DI1" s="1" t="inlineStr">
+      <c r="DJ1" s="1" t="inlineStr">
         <is>
           <t>FY2020 Q4 (D)</t>
         </is>
       </c>
-      <c r="DJ1" s="1" t="inlineStr">
+      <c r="DK1" s="1" t="inlineStr">
         <is>
           <t>FY2021 Q1 (D)</t>
         </is>
       </c>
-      <c r="DK1" s="1" t="inlineStr">
+      <c r="DL1" s="1" t="inlineStr">
         <is>
           <t>FY2021 Q2 (D)</t>
         </is>
       </c>
-      <c r="DL1" s="1" t="inlineStr">
+      <c r="DM1" s="1" t="inlineStr">
         <is>
           <t>FY2021 Q3 (D)</t>
         </is>
       </c>
-      <c r="DM1" s="1" t="inlineStr">
+      <c r="DN1" s="1" t="inlineStr">
         <is>
           <t>FY2021 Q4 (D)</t>
         </is>
       </c>
-      <c r="DN1" s="1" t="inlineStr">
+      <c r="DO1" s="1" t="inlineStr">
         <is>
           <t>FY2022 Q1 (D)</t>
         </is>
       </c>
-      <c r="DO1" s="1" t="inlineStr">
+      <c r="DP1" s="1" t="inlineStr">
         <is>
           <t>FY2022 Q2 (D)</t>
         </is>
       </c>
-      <c r="DP1" s="1" t="inlineStr">
+      <c r="DQ1" s="1" t="inlineStr">
         <is>
           <t>FY2022 Q3 (D)</t>
         </is>
       </c>
-      <c r="DQ1" s="1" t="inlineStr">
+      <c r="DR1" s="1" t="inlineStr">
         <is>
           <t>FY2022 Q4 (D)</t>
         </is>
       </c>
-      <c r="DR1" s="1" t="inlineStr">
+      <c r="DS1" s="1" t="inlineStr">
         <is>
           <t>FY2023 Q1 (D)</t>
         </is>
       </c>
-      <c r="DS1" s="1" t="inlineStr">
+      <c r="DT1" s="1" t="inlineStr">
         <is>
           <t>FY2023 Q2 (D)</t>
         </is>
       </c>
-      <c r="DT1" s="1" t="inlineStr">
+      <c r="DU1" s="1" t="inlineStr">
         <is>
           <t>FY2023 Q3 (D)</t>
         </is>
       </c>
-      <c r="DU1" s="1" t="inlineStr">
+      <c r="DV1" s="1" t="inlineStr">
         <is>
           <t>FY2023 Q4 (D)</t>
         </is>
       </c>
-      <c r="DV1" s="1" t="inlineStr">
+      <c r="DW1" s="1" t="inlineStr">
         <is>
           <t>FY2024 Q1 (D)</t>
         </is>
       </c>
-      <c r="DW1" s="1" t="inlineStr">
+      <c r="DX1" s="1" t="inlineStr">
         <is>
           <t>FY2024 Q2 (D)</t>
         </is>
       </c>
-      <c r="DX1" s="1" t="inlineStr">
+      <c r="DY1" s="1" t="inlineStr">
         <is>
           <t>FY2024 Q3 (D)</t>
         </is>
       </c>
-      <c r="DY1" s="1" t="inlineStr">
+      <c r="DZ1" s="1" t="inlineStr">
         <is>
           <t>FY2024 Q4 (D)</t>
         </is>
       </c>
-      <c r="DZ1" s="1" t="inlineStr">
+      <c r="EA1" s="1" t="inlineStr">
         <is>
           <t>FY2025 Q1 (D)</t>
         </is>
       </c>
-      <c r="EA1" s="1" t="inlineStr">
+      <c r="EB1" s="1" t="inlineStr">
         <is>
           <t>FY2025 Q2 (D)</t>
         </is>
       </c>
-      <c r="EB1" s="1" t="inlineStr">
+      <c r="EC1" s="1" t="inlineStr">
         <is>
           <t>FY2025 Q3 (D)</t>
         </is>
       </c>
-      <c r="EC1" s="1" t="inlineStr">
+      <c r="ED1" s="1" t="inlineStr">
         <is>
           <t>FY2025 Q4 (D)</t>
         </is>
@@ -1148,25 +1153,27 @@
       <c r="P2" t="inlineStr"/>
       <c r="Q2" t="inlineStr"/>
       <c r="R2" t="inlineStr"/>
-      <c r="S2" t="inlineStr"/>
+      <c r="S2" t="inlineStr">
+        <is>
+          <t>Peace and Justice Strong Institutions</t>
+        </is>
+      </c>
       <c r="T2" t="inlineStr"/>
       <c r="U2" t="inlineStr"/>
       <c r="V2" t="inlineStr"/>
       <c r="W2" t="inlineStr"/>
       <c r="X2" t="inlineStr"/>
-      <c r="Y2" t="n">
-        <v>0</v>
-      </c>
+      <c r="Y2" t="inlineStr"/>
       <c r="Z2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA2" t="n">
         <v>100</v>
       </c>
-      <c r="AA2" t="inlineStr"/>
       <c r="AB2" t="inlineStr"/>
-      <c r="AC2" s="2" t="n">
-        <v>44609</v>
-      </c>
-      <c r="AD2" t="n">
-        <v>0</v>
+      <c r="AC2" t="inlineStr"/>
+      <c r="AD2" s="2" t="n">
+        <v>44767</v>
       </c>
       <c r="AE2" t="n">
         <v>0</v>
@@ -1226,7 +1233,7 @@
         <v>0</v>
       </c>
       <c r="AX2" t="n">
-        <v>250</v>
+        <v>0</v>
       </c>
       <c r="AY2" t="n">
         <v>250</v>
@@ -1238,7 +1245,7 @@
         <v>250</v>
       </c>
       <c r="BB2" t="n">
-        <v>0</v>
+        <v>250</v>
       </c>
       <c r="BC2" t="n">
         <v>0</v>
@@ -1394,11 +1401,11 @@
         <v>0</v>
       </c>
       <c r="DB2" t="n">
+        <v>0</v>
+      </c>
+      <c r="DC2" t="n">
         <v>100</v>
       </c>
-      <c r="DC2" t="n">
-        <v>0</v>
-      </c>
       <c r="DD2" t="n">
         <v>0</v>
       </c>
@@ -1475,6 +1482,9 @@
         <v>0</v>
       </c>
       <c r="EC2" t="n">
+        <v>0</v>
+      </c>
+      <c r="ED2" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1531,25 +1541,27 @@
       <c r="P3" t="inlineStr"/>
       <c r="Q3" t="inlineStr"/>
       <c r="R3" t="inlineStr"/>
-      <c r="S3" t="inlineStr"/>
+      <c r="S3" t="inlineStr">
+        <is>
+          <t>Peace and Justice Strong Institutions</t>
+        </is>
+      </c>
       <c r="T3" t="inlineStr"/>
       <c r="U3" t="inlineStr"/>
       <c r="V3" t="inlineStr"/>
       <c r="W3" t="inlineStr"/>
       <c r="X3" t="inlineStr"/>
-      <c r="Y3" t="n">
-        <v>0</v>
-      </c>
+      <c r="Y3" t="inlineStr"/>
       <c r="Z3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA3" t="n">
         <v>2000</v>
       </c>
-      <c r="AA3" t="inlineStr"/>
       <c r="AB3" t="inlineStr"/>
-      <c r="AC3" s="2" t="n">
-        <v>44609</v>
-      </c>
-      <c r="AD3" t="n">
-        <v>0</v>
+      <c r="AC3" t="inlineStr"/>
+      <c r="AD3" s="2" t="n">
+        <v>44767</v>
       </c>
       <c r="AE3" t="n">
         <v>0</v>
@@ -1609,7 +1621,7 @@
         <v>0</v>
       </c>
       <c r="AX3" t="n">
-        <v>500</v>
+        <v>0</v>
       </c>
       <c r="AY3" t="n">
         <v>500</v>
@@ -1621,7 +1633,7 @@
         <v>500</v>
       </c>
       <c r="BB3" t="n">
-        <v>0</v>
+        <v>500</v>
       </c>
       <c r="BC3" t="n">
         <v>0</v>
@@ -1777,11 +1789,11 @@
         <v>0</v>
       </c>
       <c r="DB3" t="n">
+        <v>0</v>
+      </c>
+      <c r="DC3" t="n">
         <v>2000</v>
       </c>
-      <c r="DC3" t="n">
-        <v>0</v>
-      </c>
       <c r="DD3" t="n">
         <v>0</v>
       </c>
@@ -1858,6 +1870,9 @@
         <v>0</v>
       </c>
       <c r="EC3" t="n">
+        <v>0</v>
+      </c>
+      <c r="ED3" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1914,25 +1929,27 @@
       <c r="P4" t="inlineStr"/>
       <c r="Q4" t="inlineStr"/>
       <c r="R4" t="inlineStr"/>
-      <c r="S4" t="inlineStr"/>
+      <c r="S4" t="inlineStr">
+        <is>
+          <t>Peace and Justice Strong Institutions</t>
+        </is>
+      </c>
       <c r="T4" t="inlineStr"/>
       <c r="U4" t="inlineStr"/>
       <c r="V4" t="inlineStr"/>
       <c r="W4" t="inlineStr"/>
       <c r="X4" t="inlineStr"/>
-      <c r="Y4" t="n">
-        <v>0</v>
-      </c>
+      <c r="Y4" t="inlineStr"/>
       <c r="Z4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA4" t="n">
         <v>300</v>
       </c>
-      <c r="AA4" t="inlineStr"/>
       <c r="AB4" t="inlineStr"/>
-      <c r="AC4" s="2" t="n">
-        <v>44609</v>
-      </c>
-      <c r="AD4" t="n">
-        <v>0</v>
+      <c r="AC4" t="inlineStr"/>
+      <c r="AD4" s="2" t="n">
+        <v>44767</v>
       </c>
       <c r="AE4" t="n">
         <v>0</v>
@@ -1992,7 +2009,7 @@
         <v>0</v>
       </c>
       <c r="AX4" t="n">
-        <v>1250</v>
+        <v>0</v>
       </c>
       <c r="AY4" t="n">
         <v>1250</v>
@@ -2004,7 +2021,7 @@
         <v>1250</v>
       </c>
       <c r="BB4" t="n">
-        <v>0</v>
+        <v>1250</v>
       </c>
       <c r="BC4" t="n">
         <v>0</v>
@@ -2160,11 +2177,11 @@
         <v>0</v>
       </c>
       <c r="DB4" t="n">
+        <v>0</v>
+      </c>
+      <c r="DC4" t="n">
         <v>300</v>
       </c>
-      <c r="DC4" t="n">
-        <v>0</v>
-      </c>
       <c r="DD4" t="n">
         <v>0</v>
       </c>
@@ -2241,6 +2258,9 @@
         <v>0</v>
       </c>
       <c r="EC4" t="n">
+        <v>0</v>
+      </c>
+      <c r="ED4" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2297,25 +2317,27 @@
       <c r="P5" t="inlineStr"/>
       <c r="Q5" t="inlineStr"/>
       <c r="R5" t="inlineStr"/>
-      <c r="S5" t="inlineStr"/>
+      <c r="S5" t="inlineStr">
+        <is>
+          <t>Peace and Justice Strong Institutions</t>
+        </is>
+      </c>
       <c r="T5" t="inlineStr"/>
       <c r="U5" t="inlineStr"/>
       <c r="V5" t="inlineStr"/>
       <c r="W5" t="inlineStr"/>
       <c r="X5" t="inlineStr"/>
-      <c r="Y5" t="n">
-        <v>0</v>
-      </c>
+      <c r="Y5" t="inlineStr"/>
       <c r="Z5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA5" t="n">
         <v>400</v>
       </c>
-      <c r="AA5" t="inlineStr"/>
       <c r="AB5" t="inlineStr"/>
-      <c r="AC5" s="2" t="n">
-        <v>44609</v>
-      </c>
-      <c r="AD5" t="n">
-        <v>0</v>
+      <c r="AC5" t="inlineStr"/>
+      <c r="AD5" s="2" t="n">
+        <v>44767</v>
       </c>
       <c r="AE5" t="n">
         <v>0</v>
@@ -2375,7 +2397,7 @@
         <v>0</v>
       </c>
       <c r="AX5" t="n">
-        <v>750</v>
+        <v>0</v>
       </c>
       <c r="AY5" t="n">
         <v>750</v>
@@ -2387,7 +2409,7 @@
         <v>750</v>
       </c>
       <c r="BB5" t="n">
-        <v>0</v>
+        <v>750</v>
       </c>
       <c r="BC5" t="n">
         <v>0</v>
@@ -2543,11 +2565,11 @@
         <v>0</v>
       </c>
       <c r="DB5" t="n">
+        <v>0</v>
+      </c>
+      <c r="DC5" t="n">
         <v>400</v>
       </c>
-      <c r="DC5" t="n">
-        <v>0</v>
-      </c>
       <c r="DD5" t="n">
         <v>0</v>
       </c>
@@ -2624,6 +2646,9 @@
         <v>0</v>
       </c>
       <c r="EC5" t="n">
+        <v>0</v>
+      </c>
+      <c r="ED5" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2680,25 +2705,27 @@
       <c r="P6" t="inlineStr"/>
       <c r="Q6" t="inlineStr"/>
       <c r="R6" t="inlineStr"/>
-      <c r="S6" t="inlineStr"/>
+      <c r="S6" t="inlineStr">
+        <is>
+          <t>Peace and Justice Strong Institutions</t>
+        </is>
+      </c>
       <c r="T6" t="inlineStr"/>
       <c r="U6" t="inlineStr"/>
       <c r="V6" t="inlineStr"/>
       <c r="W6" t="inlineStr"/>
       <c r="X6" t="inlineStr"/>
-      <c r="Y6" t="n">
-        <v>0</v>
-      </c>
+      <c r="Y6" t="inlineStr"/>
       <c r="Z6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA6" t="n">
         <v>5000</v>
       </c>
-      <c r="AA6" t="inlineStr"/>
       <c r="AB6" t="inlineStr"/>
-      <c r="AC6" s="2" t="n">
-        <v>44609</v>
-      </c>
-      <c r="AD6" t="n">
-        <v>0</v>
+      <c r="AC6" t="inlineStr"/>
+      <c r="AD6" s="2" t="n">
+        <v>44767</v>
       </c>
       <c r="AE6" t="n">
         <v>0</v>
@@ -2758,7 +2785,7 @@
         <v>0</v>
       </c>
       <c r="AX6" t="n">
-        <v>5000</v>
+        <v>0</v>
       </c>
       <c r="AY6" t="n">
         <v>5000</v>
@@ -2770,7 +2797,7 @@
         <v>5000</v>
       </c>
       <c r="BB6" t="n">
-        <v>0</v>
+        <v>5000</v>
       </c>
       <c r="BC6" t="n">
         <v>0</v>
@@ -2926,11 +2953,11 @@
         <v>0</v>
       </c>
       <c r="DB6" t="n">
+        <v>0</v>
+      </c>
+      <c r="DC6" t="n">
         <v>5000</v>
       </c>
-      <c r="DC6" t="n">
-        <v>0</v>
-      </c>
       <c r="DD6" t="n">
         <v>0</v>
       </c>
@@ -3007,6 +3034,9 @@
         <v>0</v>
       </c>
       <c r="EC6" t="n">
+        <v>0</v>
+      </c>
+      <c r="ED6" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3063,25 +3093,27 @@
       <c r="P7" t="inlineStr"/>
       <c r="Q7" t="inlineStr"/>
       <c r="R7" t="inlineStr"/>
-      <c r="S7" t="inlineStr"/>
+      <c r="S7" t="inlineStr">
+        <is>
+          <t>Peace and Justice Strong Institutions</t>
+        </is>
+      </c>
       <c r="T7" t="inlineStr"/>
       <c r="U7" t="inlineStr"/>
       <c r="V7" t="inlineStr"/>
       <c r="W7" t="inlineStr"/>
       <c r="X7" t="inlineStr"/>
-      <c r="Y7" t="n">
-        <v>0</v>
-      </c>
+      <c r="Y7" t="inlineStr"/>
       <c r="Z7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA7" t="n">
         <v>100</v>
       </c>
-      <c r="AA7" t="inlineStr"/>
       <c r="AB7" t="inlineStr"/>
-      <c r="AC7" s="2" t="n">
-        <v>44609</v>
-      </c>
-      <c r="AD7" t="n">
-        <v>0</v>
+      <c r="AC7" t="inlineStr"/>
+      <c r="AD7" s="2" t="n">
+        <v>44767</v>
       </c>
       <c r="AE7" t="n">
         <v>0</v>
@@ -3141,7 +3173,7 @@
         <v>0</v>
       </c>
       <c r="AX7" t="n">
-        <v>2500</v>
+        <v>0</v>
       </c>
       <c r="AY7" t="n">
         <v>2500</v>
@@ -3153,7 +3185,7 @@
         <v>2500</v>
       </c>
       <c r="BB7" t="n">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="BC7" t="n">
         <v>0</v>
@@ -3309,11 +3341,11 @@
         <v>0</v>
       </c>
       <c r="DB7" t="n">
+        <v>0</v>
+      </c>
+      <c r="DC7" t="n">
         <v>100</v>
       </c>
-      <c r="DC7" t="n">
-        <v>0</v>
-      </c>
       <c r="DD7" t="n">
         <v>0</v>
       </c>
@@ -3390,6 +3422,9 @@
         <v>0</v>
       </c>
       <c r="EC7" t="n">
+        <v>0</v>
+      </c>
+      <c r="ED7" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3446,25 +3481,27 @@
       <c r="P8" t="inlineStr"/>
       <c r="Q8" t="inlineStr"/>
       <c r="R8" t="inlineStr"/>
-      <c r="S8" t="inlineStr"/>
+      <c r="S8" t="inlineStr">
+        <is>
+          <t>Peace and Justice Strong Institutions</t>
+        </is>
+      </c>
       <c r="T8" t="inlineStr"/>
       <c r="U8" t="inlineStr"/>
       <c r="V8" t="inlineStr"/>
       <c r="W8" t="inlineStr"/>
       <c r="X8" t="inlineStr"/>
-      <c r="Y8" t="n">
-        <v>0</v>
-      </c>
+      <c r="Y8" t="inlineStr"/>
       <c r="Z8" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA8" t="n">
         <v>200</v>
       </c>
-      <c r="AA8" t="inlineStr"/>
       <c r="AB8" t="inlineStr"/>
-      <c r="AC8" s="2" t="n">
-        <v>44609</v>
-      </c>
-      <c r="AD8" t="n">
-        <v>0</v>
+      <c r="AC8" t="inlineStr"/>
+      <c r="AD8" s="2" t="n">
+        <v>44767</v>
       </c>
       <c r="AE8" t="n">
         <v>0</v>
@@ -3524,7 +3561,7 @@
         <v>0</v>
       </c>
       <c r="AX8" t="n">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AY8" t="n">
         <v>1000</v>
@@ -3536,7 +3573,7 @@
         <v>1000</v>
       </c>
       <c r="BB8" t="n">
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="BC8" t="n">
         <v>0</v>
@@ -3692,11 +3729,11 @@
         <v>0</v>
       </c>
       <c r="DB8" t="n">
+        <v>0</v>
+      </c>
+      <c r="DC8" t="n">
         <v>200</v>
       </c>
-      <c r="DC8" t="n">
-        <v>0</v>
-      </c>
       <c r="DD8" t="n">
         <v>0</v>
       </c>
@@ -3773,6 +3810,9 @@
         <v>0</v>
       </c>
       <c r="EC8" t="n">
+        <v>0</v>
+      </c>
+      <c r="ED8" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3829,25 +3869,27 @@
       <c r="P9" t="inlineStr"/>
       <c r="Q9" t="inlineStr"/>
       <c r="R9" t="inlineStr"/>
-      <c r="S9" t="inlineStr"/>
+      <c r="S9" t="inlineStr">
+        <is>
+          <t>Peace and Justice Strong Institutions</t>
+        </is>
+      </c>
       <c r="T9" t="inlineStr"/>
       <c r="U9" t="inlineStr"/>
       <c r="V9" t="inlineStr"/>
       <c r="W9" t="inlineStr"/>
       <c r="X9" t="inlineStr"/>
-      <c r="Y9" t="n">
-        <v>0</v>
-      </c>
+      <c r="Y9" t="inlineStr"/>
       <c r="Z9" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA9" t="n">
         <v>700</v>
       </c>
-      <c r="AA9" t="inlineStr"/>
       <c r="AB9" t="inlineStr"/>
-      <c r="AC9" s="2" t="n">
-        <v>44609</v>
-      </c>
-      <c r="AD9" t="n">
-        <v>0</v>
+      <c r="AC9" t="inlineStr"/>
+      <c r="AD9" s="2" t="n">
+        <v>44767</v>
       </c>
       <c r="AE9" t="n">
         <v>0</v>
@@ -3907,7 +3949,7 @@
         <v>0</v>
       </c>
       <c r="AX9" t="n">
-        <v>625</v>
+        <v>0</v>
       </c>
       <c r="AY9" t="n">
         <v>625</v>
@@ -3919,7 +3961,7 @@
         <v>625</v>
       </c>
       <c r="BB9" t="n">
-        <v>0</v>
+        <v>625</v>
       </c>
       <c r="BC9" t="n">
         <v>0</v>
@@ -4075,11 +4117,11 @@
         <v>0</v>
       </c>
       <c r="DB9" t="n">
+        <v>0</v>
+      </c>
+      <c r="DC9" t="n">
         <v>700</v>
       </c>
-      <c r="DC9" t="n">
-        <v>0</v>
-      </c>
       <c r="DD9" t="n">
         <v>0</v>
       </c>
@@ -4156,6 +4198,9 @@
         <v>0</v>
       </c>
       <c r="EC9" t="n">
+        <v>0</v>
+      </c>
+      <c r="ED9" t="n">
         <v>0</v>
       </c>
     </row>
@@ -4212,25 +4257,27 @@
       <c r="P10" t="inlineStr"/>
       <c r="Q10" t="inlineStr"/>
       <c r="R10" t="inlineStr"/>
-      <c r="S10" t="inlineStr"/>
+      <c r="S10" t="inlineStr">
+        <is>
+          <t>Peace and Justice Strong Institutions</t>
+        </is>
+      </c>
       <c r="T10" t="inlineStr"/>
       <c r="U10" t="inlineStr"/>
       <c r="V10" t="inlineStr"/>
       <c r="W10" t="inlineStr"/>
       <c r="X10" t="inlineStr"/>
-      <c r="Y10" t="n">
-        <v>0</v>
-      </c>
+      <c r="Y10" t="inlineStr"/>
       <c r="Z10" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA10" t="n">
         <v>450</v>
       </c>
-      <c r="AA10" t="inlineStr"/>
       <c r="AB10" t="inlineStr"/>
-      <c r="AC10" s="2" t="n">
-        <v>44609</v>
-      </c>
-      <c r="AD10" t="n">
-        <v>0</v>
+      <c r="AC10" t="inlineStr"/>
+      <c r="AD10" s="2" t="n">
+        <v>44767</v>
       </c>
       <c r="AE10" t="n">
         <v>0</v>
@@ -4290,7 +4337,7 @@
         <v>0</v>
       </c>
       <c r="AX10" t="n">
-        <v>375</v>
+        <v>0</v>
       </c>
       <c r="AY10" t="n">
         <v>375</v>
@@ -4302,7 +4349,7 @@
         <v>375</v>
       </c>
       <c r="BB10" t="n">
-        <v>0</v>
+        <v>375</v>
       </c>
       <c r="BC10" t="n">
         <v>0</v>
@@ -4458,11 +4505,11 @@
         <v>0</v>
       </c>
       <c r="DB10" t="n">
+        <v>0</v>
+      </c>
+      <c r="DC10" t="n">
         <v>450</v>
       </c>
-      <c r="DC10" t="n">
-        <v>0</v>
-      </c>
       <c r="DD10" t="n">
         <v>0</v>
       </c>
@@ -4539,6 +4586,9 @@
         <v>0</v>
       </c>
       <c r="EC10" t="n">
+        <v>0</v>
+      </c>
+      <c r="ED10" t="n">
         <v>0</v>
       </c>
     </row>
@@ -4595,25 +4645,27 @@
       <c r="P11" t="inlineStr"/>
       <c r="Q11" t="inlineStr"/>
       <c r="R11" t="inlineStr"/>
-      <c r="S11" t="inlineStr"/>
+      <c r="S11" t="inlineStr">
+        <is>
+          <t>Peace and Justice Strong Institutions</t>
+        </is>
+      </c>
       <c r="T11" t="inlineStr"/>
       <c r="U11" t="inlineStr"/>
       <c r="V11" t="inlineStr"/>
       <c r="W11" t="inlineStr"/>
       <c r="X11" t="inlineStr"/>
-      <c r="Y11" t="n">
-        <v>0</v>
-      </c>
+      <c r="Y11" t="inlineStr"/>
       <c r="Z11" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA11" t="n">
         <v>1300</v>
       </c>
-      <c r="AA11" t="inlineStr"/>
       <c r="AB11" t="inlineStr"/>
-      <c r="AC11" s="2" t="n">
-        <v>44609</v>
-      </c>
-      <c r="AD11" t="n">
-        <v>0</v>
+      <c r="AC11" t="inlineStr"/>
+      <c r="AD11" s="2" t="n">
+        <v>44767</v>
       </c>
       <c r="AE11" t="n">
         <v>0</v>
@@ -4673,7 +4725,7 @@
         <v>0</v>
       </c>
       <c r="AX11" t="n">
-        <v>750</v>
+        <v>0</v>
       </c>
       <c r="AY11" t="n">
         <v>750</v>
@@ -4685,7 +4737,7 @@
         <v>750</v>
       </c>
       <c r="BB11" t="n">
-        <v>0</v>
+        <v>750</v>
       </c>
       <c r="BC11" t="n">
         <v>0</v>
@@ -4841,11 +4893,11 @@
         <v>0</v>
       </c>
       <c r="DB11" t="n">
+        <v>0</v>
+      </c>
+      <c r="DC11" t="n">
         <v>1300</v>
       </c>
-      <c r="DC11" t="n">
-        <v>0</v>
-      </c>
       <c r="DD11" t="n">
         <v>0</v>
       </c>
@@ -4922,6 +4974,9 @@
         <v>0</v>
       </c>
       <c r="EC11" t="n">
+        <v>0</v>
+      </c>
+      <c r="ED11" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>